<commit_message>
week of 31 October
</commit_message>
<xml_diff>
--- a/data/input/base_financing_cds.xlsx
+++ b/data/input/base_financing_cds.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg-my.sharepoint.com/personal/brooksd_who_int/Documents/Documents/GitHub/covid19_vaccination_analysis/data/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg-my.sharepoint.com/personal/panlilioj_who_int/Documents/covid19_vaccination_analysis/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="13_ncr:1_{26E979B5-FA10-4638-B812-BC8073066A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{364BF911-6B67-4011-92C6-309C591AD5C2}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{26E979B5-FA10-4638-B812-BC8073066A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDD1422A-CFCF-4956-9672-D63CAB2CD968}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{FD644F38-BFEB-4730-9E59-BCD9CF33A41F}"/>
+    <workbookView xWindow="28690" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{FD644F38-BFEB-4730-9E59-BCD9CF33A41F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="10" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,6 +35,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -360,36 +362,42 @@
     <t xml:space="preserve">Sum of Amount approved </t>
   </si>
   <si>
+    <t>ISO</t>
+  </si>
+  <si>
+    <t>SYR</t>
+  </si>
+  <si>
     <t>AFG</t>
   </si>
   <si>
+    <t>BFA</t>
+  </si>
+  <si>
+    <t>CAF</t>
+  </si>
+  <si>
+    <t>TCD</t>
+  </si>
+  <si>
+    <t>COD</t>
+  </si>
+  <si>
     <t>ETH</t>
   </si>
   <si>
     <t>GHA</t>
   </si>
   <si>
+    <t>GIN</t>
+  </si>
+  <si>
+    <t>HTI</t>
+  </si>
+  <si>
     <t>KEN</t>
   </si>
   <si>
-    <t>BFA</t>
-  </si>
-  <si>
-    <t>CAF</t>
-  </si>
-  <si>
-    <t>TCD</t>
-  </si>
-  <si>
-    <t>COD</t>
-  </si>
-  <si>
-    <t>GIN</t>
-  </si>
-  <si>
-    <t>HTI</t>
-  </si>
-  <si>
     <t>MWI</t>
   </si>
   <si>
@@ -414,9 +422,6 @@
     <t>SDN</t>
   </si>
   <si>
-    <t>SYR</t>
-  </si>
-  <si>
     <t>TZA</t>
   </si>
   <si>
@@ -441,19 +446,16 @@
     <t>GMB</t>
   </si>
   <si>
+    <t>GNB</t>
+  </si>
+  <si>
+    <t>MDG</t>
+  </si>
+  <si>
     <t>MLI</t>
   </si>
   <si>
     <t>SEN</t>
-  </si>
-  <si>
-    <t>GNB</t>
-  </si>
-  <si>
-    <t>MDG</t>
-  </si>
-  <si>
-    <t>ISO</t>
   </si>
 </sst>
 </file>
@@ -461,15 +463,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="9">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yyyy;@"/>
-    <numFmt numFmtId="168" formatCode="[$-409]dd\-mmm\-yy;@"/>
-    <numFmt numFmtId="169" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="170" formatCode="_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="169" formatCode="[$-409]dd\-mmm\-yy;@"/>
+    <numFmt numFmtId="170" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="171" formatCode="_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="172" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -731,7 +733,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -743,7 +745,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -793,7 +795,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -820,7 +822,7 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="5" fillId="12" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="168" fontId="6" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="6" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -837,18 +839,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -863,19 +865,19 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="40" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -893,10 +895,10 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="6" fillId="13" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -909,7 +911,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="40% - Accent4 5" xfId="4" xr:uid="{BBE1C5CD-EB81-46A5-A1EB-6EEB64CB90EF}"/>
@@ -959,7 +961,7 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="171" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="172" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1664,7 +1666,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C9206A13-E1F8-4BA4-9E83-D2C707B1EEF4}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C9206A13-E1F8-4BA4-9E83-D2C707B1EEF4}" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:C36" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
@@ -1837,7 +1839,7 @@
   </colItems>
   <dataFields count="2">
     <dataField name="Sum of Amount approved " fld="3" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Amount disbursed " fld="5" baseField="0" baseItem="0" numFmtId="171"/>
+    <dataField name="Sum of Amount disbursed " fld="5" baseField="0" baseItem="0" numFmtId="172"/>
   </dataFields>
   <formats count="1">
     <format dxfId="4">
@@ -2179,14 +2181,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.9296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.06640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="77" t="s">
         <v>72</v>
       </c>
@@ -2197,7 +2199,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="78" t="s">
         <v>8</v>
       </c>
@@ -2208,7 +2210,7 @@
         <v>19302055</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="78" t="s">
         <v>11</v>
       </c>
@@ -2219,7 +2221,7 @@
         <v>7171272.7999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="78" t="s">
         <v>56</v>
       </c>
@@ -2230,7 +2232,7 @@
         <v>5427618</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="78" t="s">
         <v>13</v>
       </c>
@@ -2241,7 +2243,7 @@
         <v>1396005</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="78" t="s">
         <v>16</v>
       </c>
@@ -2252,7 +2254,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="78" t="s">
         <v>19</v>
       </c>
@@ -2263,7 +2265,7 @@
         <v>28514291.93</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="78" t="s">
         <v>57</v>
       </c>
@@ -2274,7 +2276,7 @@
         <v>2628307</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="78" t="s">
         <v>58</v>
       </c>
@@ -2285,7 +2287,7 @@
         <v>978421</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="78" t="s">
         <v>21</v>
       </c>
@@ -2296,7 +2298,7 @@
         <v>23138107.899999999</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="78" t="s">
         <v>59</v>
       </c>
@@ -2307,7 +2309,7 @@
         <v>977007</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="78" t="s">
         <v>24</v>
       </c>
@@ -2318,7 +2320,7 @@
         <v>9659426.370000001</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="78" t="s">
         <v>26</v>
       </c>
@@ -2329,7 +2331,7 @@
         <v>2304800</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="78" t="s">
         <v>60</v>
       </c>
@@ -2340,7 +2342,7 @@
         <v>978460</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="78" t="s">
         <v>29</v>
       </c>
@@ -2351,7 +2353,7 @@
         <v>2138482.09</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="78" t="s">
         <v>32</v>
       </c>
@@ -2362,7 +2364,7 @@
         <v>6035928</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="78" t="s">
         <v>61</v>
       </c>
@@ -2373,7 +2375,7 @@
         <v>4064028</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="78" t="s">
         <v>35</v>
       </c>
@@ -2384,7 +2386,7 @@
         <v>1993648.65</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="78" t="s">
         <v>62</v>
       </c>
@@ -2395,7 +2397,7 @@
         <v>3625429</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="78" t="s">
         <v>37</v>
       </c>
@@ -2406,7 +2408,7 @@
         <v>6475917</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="78" t="s">
         <v>38</v>
       </c>
@@ -2417,7 +2419,7 @@
         <v>37437345.109999999</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="78" t="s">
         <v>40</v>
       </c>
@@ -2428,7 +2430,7 @@
         <v>1560177.25</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="78" t="s">
         <v>63</v>
       </c>
@@ -2439,7 +2441,7 @@
         <v>1380115</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="78" t="s">
         <v>41</v>
       </c>
@@ -2450,7 +2452,7 @@
         <v>2944971</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="78" t="s">
         <v>43</v>
       </c>
@@ -2461,7 +2463,7 @@
         <v>10652720.32</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="78" t="s">
         <v>45</v>
       </c>
@@ -2472,7 +2474,7 @@
         <v>5446372</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="78" t="s">
         <v>46</v>
       </c>
@@ -2483,7 +2485,7 @@
         <v>9296766</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="78" t="s">
         <v>64</v>
       </c>
@@ -2494,7 +2496,7 @@
         <v>2730325</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" s="78" t="s">
         <v>47</v>
       </c>
@@ -2505,7 +2507,7 @@
         <v>4692089.46</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" s="78" t="s">
         <v>48</v>
       </c>
@@ -2516,7 +2518,7 @@
         <v>1652677</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="78" t="s">
         <v>49</v>
       </c>
@@ -2527,7 +2529,7 @@
         <v>3301114</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="78" t="s">
         <v>50</v>
       </c>
@@ -2538,7 +2540,7 @@
         <v>21778540</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" s="78" t="s">
         <v>51</v>
       </c>
@@ -2549,7 +2551,7 @@
         <v>6554186</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" s="78" t="s">
         <v>52</v>
       </c>
@@ -2560,7 +2562,7 @@
         <v>4283508</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" s="78" t="s">
         <v>54</v>
       </c>
@@ -2571,7 +2573,7 @@
         <v>8542014.6500000004</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="78" t="s">
         <v>73</v>
       </c>
@@ -2592,27 +2594,27 @@
   <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="19.25" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="22.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="1" max="2" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.46484375" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
     <col min="6" max="6" width="19" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="69.42578125" customWidth="1"/>
-    <col min="9" max="9" width="70.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="69.46484375" customWidth="1"/>
+    <col min="9" max="9" width="70.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="58.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>107</v>
+    <row r="1" spans="1:9" ht="58.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>0</v>
@@ -2639,9 +2641,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="48" customFormat="1" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
-        <v>76</v>
+    <row r="2" spans="1:9" s="48" customFormat="1" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="11" t="s">
+        <v>78</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>8</v>
@@ -2663,9 +2665,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>80</v>
+    <row r="3" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>11</v>
@@ -2687,9 +2689,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>81</v>
+    <row r="4" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="11" t="s">
+        <v>80</v>
       </c>
       <c r="B4" s="52" t="s">
         <v>13</v>
@@ -2712,9 +2714,9 @@
       </c>
       <c r="I4" s="41"/>
     </row>
-    <row r="5" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>82</v>
+    <row r="5" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="11" t="s">
+        <v>81</v>
       </c>
       <c r="B5" s="52" t="s">
         <v>16</v>
@@ -2733,9 +2735,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>83</v>
+    <row r="6" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="11" t="s">
+        <v>82</v>
       </c>
       <c r="B6" s="52" t="s">
         <v>19</v>
@@ -2757,9 +2759,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>77</v>
+    <row r="7" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="11" t="s">
+        <v>83</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>21</v>
@@ -2781,9 +2783,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>77</v>
+    <row r="8" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="11" t="s">
+        <v>83</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>21</v>
@@ -2807,9 +2809,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>78</v>
+    <row r="9" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>24</v>
@@ -2832,9 +2834,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>84</v>
+    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="11" t="s">
+        <v>85</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>26</v>
@@ -2855,9 +2857,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>85</v>
+    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="11" t="s">
+        <v>86</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>29</v>
@@ -2876,9 +2878,9 @@
       </c>
       <c r="I11" s="38"/>
     </row>
-    <row r="12" spans="1:9" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>79</v>
+    <row r="12" spans="1:9" ht="34.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>32</v>
@@ -2900,9 +2902,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>79</v>
+    <row r="13" spans="1:9" ht="34.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>32</v>
@@ -2920,9 +2922,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>86</v>
+    <row r="14" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="11" t="s">
+        <v>88</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>35</v>
@@ -2944,9 +2946,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>86</v>
+    <row r="15" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="11" t="s">
+        <v>88</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>35</v>
@@ -2966,9 +2968,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>87</v>
+    <row r="16" spans="1:9" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="11" t="s">
+        <v>89</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>37</v>
@@ -2990,9 +2992,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>88</v>
+    <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="11" t="s">
+        <v>90</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>38</v>
@@ -3016,9 +3018,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>88</v>
+    <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="11" t="s">
+        <v>90</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>38</v>
@@ -3042,9 +3044,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>89</v>
+    <row r="19" spans="1:8" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="11" t="s">
+        <v>91</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>40</v>
@@ -3067,9 +3069,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>90</v>
+    <row r="20" spans="1:8" ht="28.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="11" t="s">
+        <v>92</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>41</v>
@@ -3093,9 +3095,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>91</v>
+    <row r="21" spans="1:8" ht="40.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="11" t="s">
+        <v>93</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>43</v>
@@ -3120,9 +3122,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>92</v>
+    <row r="22" spans="1:8" ht="34.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="11" t="s">
+        <v>94</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>45</v>
@@ -3146,9 +3148,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>93</v>
+    <row r="23" spans="1:8" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="11" t="s">
+        <v>95</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>46</v>
@@ -3172,9 +3174,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>94</v>
+    <row r="24" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>47</v>
@@ -3196,9 +3198,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>94</v>
+    <row r="25" spans="1:8" ht="45.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>48</v>
@@ -3221,9 +3223,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>94</v>
+    <row r="26" spans="1:8" ht="45.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>49</v>
@@ -3245,9 +3247,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>95</v>
+    <row r="27" spans="1:8" ht="40.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>50</v>
@@ -3269,9 +3271,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>95</v>
+    <row r="28" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>50</v>
@@ -3293,9 +3295,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>96</v>
+    <row r="29" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="11" t="s">
+        <v>97</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>51</v>
@@ -3317,9 +3319,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>97</v>
+    <row r="30" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="11" t="s">
+        <v>98</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>52</v>
@@ -3339,9 +3341,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>98</v>
+    <row r="31" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="11" t="s">
+        <v>99</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>54</v>
@@ -3363,9 +3365,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>76</v>
+    <row r="32" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="11" t="s">
+        <v>78</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>8</v>
@@ -3388,9 +3390,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>80</v>
+    <row r="33" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>11</v>
@@ -3412,9 +3414,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>99</v>
+    <row r="34" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="11" t="s">
+        <v>100</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>56</v>
@@ -3437,9 +3439,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>81</v>
+    <row r="35" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="11" t="s">
+        <v>80</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>13</v>
@@ -3461,9 +3463,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>82</v>
+    <row r="36" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="11" t="s">
+        <v>81</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>16</v>
@@ -3486,9 +3488,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>83</v>
+    <row r="37" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="11" t="s">
+        <v>82</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>19</v>
@@ -3511,9 +3513,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>100</v>
+    <row r="38" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A38" s="11" t="s">
+        <v>101</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>57</v>
@@ -3535,9 +3537,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>101</v>
+    <row r="39" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="11" t="s">
+        <v>102</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>58</v>
@@ -3560,9 +3562,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>77</v>
+    <row r="40" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="11" t="s">
+        <v>83</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>21</v>
@@ -3585,9 +3587,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>102</v>
+    <row r="41" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>59</v>
@@ -3609,9 +3611,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>78</v>
+    <row r="42" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>24</v>
@@ -3634,9 +3636,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>84</v>
+    <row r="43" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A43" s="11" t="s">
+        <v>85</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>26</v>
@@ -3659,9 +3661,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>105</v>
+    <row r="44" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="11" t="s">
+        <v>104</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>60</v>
@@ -3683,9 +3685,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>85</v>
+    <row r="45" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="11" t="s">
+        <v>86</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>29</v>
@@ -3708,9 +3710,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>79</v>
+    <row r="46" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A46" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>32</v>
@@ -3733,9 +3735,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>106</v>
+    <row r="47" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="11" t="s">
+        <v>105</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>61</v>
@@ -3758,9 +3760,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>86</v>
+    <row r="48" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="11" t="s">
+        <v>88</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>35</v>
@@ -3783,9 +3785,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>103</v>
+    <row r="49" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="11" t="s">
+        <v>106</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>62</v>
@@ -3808,9 +3810,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>87</v>
+    <row r="50" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="11" t="s">
+        <v>89</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>37</v>
@@ -3832,9 +3834,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>88</v>
+    <row r="51" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="11" t="s">
+        <v>90</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>38</v>
@@ -3857,9 +3859,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>89</v>
+    <row r="52" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A52" s="11" t="s">
+        <v>91</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>40</v>
@@ -3881,9 +3883,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>104</v>
+    <row r="53" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A53" s="11" t="s">
+        <v>107</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>63</v>
@@ -3905,9 +3907,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>90</v>
+    <row r="54" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A54" s="11" t="s">
+        <v>92</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>41</v>
@@ -3930,9 +3932,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>91</v>
+    <row r="55" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A55" s="11" t="s">
+        <v>93</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>43</v>
@@ -3955,9 +3957,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>92</v>
+    <row r="56" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A56" s="11" t="s">
+        <v>94</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>45</v>
@@ -3980,9 +3982,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>93</v>
+    <row r="57" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A57" s="11" t="s">
+        <v>95</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>46</v>
@@ -4005,9 +4007,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>94</v>
+    <row r="58" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A58" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="B58" s="12" t="s">
         <v>64</v>
@@ -4030,9 +4032,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>95</v>
+    <row r="59" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A59" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>50</v>
@@ -4054,9 +4056,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>96</v>
+    <row r="60" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A60" s="11" t="s">
+        <v>97</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>51</v>
@@ -4079,9 +4081,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>97</v>
+    <row r="61" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A61" s="11" t="s">
+        <v>98</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>52</v>
@@ -4104,9 +4106,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>98</v>
+    <row r="62" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A62" s="11" t="s">
+        <v>99</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>54</v>
@@ -4129,7 +4131,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="G63" s="41"/>
     </row>
   </sheetData>
@@ -4173,54 +4175,54 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="43.7109375" customWidth="1"/>
+    <col min="1" max="1" width="43.6640625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="27" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="20"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="28" t="s">
         <v>66</v>
       </c>
       <c r="B3" s="21"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="29" t="s">
         <v>67</v>
       </c>
       <c r="B4" s="26"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="30" t="s">
         <v>68</v>
       </c>
       <c r="B5" s="22"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="31" t="s">
         <v>69</v>
       </c>
       <c r="B6" s="24"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="32" t="s">
         <v>70</v>
       </c>
       <c r="B7" s="23"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="33" t="s">
         <v>71</v>
       </c>
@@ -4245,6 +4247,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001F87334A6AC30D4EA6021977FA7E2445" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="13eff9136b4917bb459ad9c1db870f6d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b370a6fa-a798-42e0-969d-19c284d8683f" xmlns:ns3="62ca1376-8bea-4949-825e-fec085c3924e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="60e7197df19c7150b1ba0c3bfe00adf4" ns2:_="" ns3:_="">
     <xsd:import namespace="b370a6fa-a798-42e0-969d-19c284d8683f"/>
@@ -4461,12 +4469,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DDCF067-268F-4A3C-A288-B4575E68AABA}">
   <ds:schemaRefs>
@@ -4476,6 +4478,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{752D7A7F-0D65-4907-85A4-76807BF1350E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d0706217-df7c-4bf4-936d-b09aa3b837af"/>
+    <ds:schemaRef ds:uri="5c2490db-6e42-4989-a0fb-d6ff54a6a7de"/>
+    <ds:schemaRef ds:uri="55894003-98dc-4f3e-8669-85b90bdbcc8c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D681DB6D-9136-4740-BD99-737079D2FCBE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4492,16 +4506,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{752D7A7F-0D65-4907-85A4-76807BF1350E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d0706217-df7c-4bf4-936d-b09aa3b837af"/>
-    <ds:schemaRef ds:uri="5c2490db-6e42-4989-a0fb-d6ff54a6a7de"/>
-    <ds:schemaRef ds:uri="55894003-98dc-4f3e-8669-85b90bdbcc8c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Revise - 11 October 2022
</commit_message>
<xml_diff>
--- a/data/input/base_financing_cds.xlsx
+++ b/data/input/base_financing_cds.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
-  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg-my.sharepoint.com/personal/panlilioj_who_int/Documents/covid19_vaccination_analysis/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{26E979B5-FA10-4638-B812-BC8073066A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDD1422A-CFCF-4956-9672-D63CAB2CD968}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{26E979B5-FA10-4638-B812-BC8073066A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{811E209E-4D9A-416A-82DE-D29085A772AB}"/>
   <bookViews>
     <workbookView xWindow="28690" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{FD644F38-BFEB-4730-9E59-BCD9CF33A41F}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -365,97 +365,97 @@
     <t>ISO</t>
   </si>
   <si>
+    <t>AFG</t>
+  </si>
+  <si>
+    <t>BFA</t>
+  </si>
+  <si>
+    <t>CAF</t>
+  </si>
+  <si>
+    <t>TCD</t>
+  </si>
+  <si>
+    <t>ETH</t>
+  </si>
+  <si>
+    <t>GHA</t>
+  </si>
+  <si>
+    <t>GIN</t>
+  </si>
+  <si>
+    <t>HTI</t>
+  </si>
+  <si>
+    <t>KEN</t>
+  </si>
+  <si>
+    <t>MWI</t>
+  </si>
+  <si>
+    <t>NER</t>
+  </si>
+  <si>
+    <t>NGA</t>
+  </si>
+  <si>
+    <t>PNG</t>
+  </si>
+  <si>
+    <t>SLE</t>
+  </si>
+  <si>
+    <t>SOM</t>
+  </si>
+  <si>
+    <t>SSD</t>
+  </si>
+  <si>
+    <t>SDN</t>
+  </si>
+  <si>
+    <t>UGA</t>
+  </si>
+  <si>
+    <t>ZMB</t>
+  </si>
+  <si>
+    <t>CMR</t>
+  </si>
+  <si>
+    <t>DJI</t>
+  </si>
+  <si>
+    <t>GNB</t>
+  </si>
+  <si>
+    <t>MDG</t>
+  </si>
+  <si>
+    <t>MLI</t>
+  </si>
+  <si>
+    <t>SEN</t>
+  </si>
+  <si>
     <t>SYR</t>
   </si>
   <si>
-    <t>AFG</t>
-  </si>
-  <si>
-    <t>BFA</t>
-  </si>
-  <si>
-    <t>CAF</t>
-  </si>
-  <si>
-    <t>TCD</t>
+    <t>TZA</t>
+  </si>
+  <si>
+    <t>YEM</t>
+  </si>
+  <si>
+    <t>GMB</t>
   </si>
   <si>
     <t>COD</t>
   </si>
   <si>
-    <t>ETH</t>
-  </si>
-  <si>
-    <t>GHA</t>
-  </si>
-  <si>
-    <t>GIN</t>
-  </si>
-  <si>
-    <t>HTI</t>
-  </si>
-  <si>
-    <t>KEN</t>
-  </si>
-  <si>
-    <t>MWI</t>
-  </si>
-  <si>
-    <t>NER</t>
-  </si>
-  <si>
-    <t>NGA</t>
-  </si>
-  <si>
-    <t>PNG</t>
-  </si>
-  <si>
-    <t>SLE</t>
-  </si>
-  <si>
-    <t>SOM</t>
-  </si>
-  <si>
-    <t>SSD</t>
-  </si>
-  <si>
-    <t>SDN</t>
-  </si>
-  <si>
-    <t>TZA</t>
-  </si>
-  <si>
-    <t>UGA</t>
-  </si>
-  <si>
-    <t>YEM</t>
-  </si>
-  <si>
-    <t>ZMB</t>
-  </si>
-  <si>
-    <t>CMR</t>
-  </si>
-  <si>
     <t>CIV</t>
-  </si>
-  <si>
-    <t>DJI</t>
-  </si>
-  <si>
-    <t>GMB</t>
-  </si>
-  <si>
-    <t>GNB</t>
-  </si>
-  <si>
-    <t>MDG</t>
-  </si>
-  <si>
-    <t>MLI</t>
-  </si>
-  <si>
-    <t>SEN</t>
   </si>
 </sst>
 </file>
@@ -738,7 +738,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -755,9 +755,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -780,7 +777,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -819,13 +815,10 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="12" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="169" fontId="6" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -850,7 +843,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -862,9 +854,6 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="6" fillId="13" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -880,9 +869,6 @@
     <xf numFmtId="169" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -895,16 +881,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="13" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="40" fontId="0" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="40" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -912,6 +891,54 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="12" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="12" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="40% - Accent4 5" xfId="4" xr:uid="{BBE1C5CD-EB81-46A5-A1EB-6EEB64CB90EF}"/>
@@ -974,6 +1001,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1666,7 +1697,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C9206A13-E1F8-4BA4-9E83-D2C707B1EEF4}" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C9206A13-E1F8-4BA4-9E83-D2C707B1EEF4}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:C36" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
@@ -2189,7 +2220,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="65" t="s">
         <v>72</v>
       </c>
       <c r="B1" t="s">
@@ -2200,387 +2231,387 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="79">
+      <c r="B2" s="67">
         <v>19794913</v>
       </c>
-      <c r="C2" s="79">
+      <c r="C2" s="67">
         <v>19302055</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="79">
+      <c r="B3" s="67">
         <v>11402242</v>
       </c>
-      <c r="C3" s="79">
+      <c r="C3" s="67">
         <v>7171272.7999999998</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="79">
+      <c r="B4" s="67">
         <v>5507618</v>
       </c>
-      <c r="C4" s="79">
+      <c r="C4" s="67">
         <v>5427618</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="79">
+      <c r="B5" s="67">
         <v>2880301</v>
       </c>
-      <c r="C5" s="79">
+      <c r="C5" s="67">
         <v>1396005</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="79">
+      <c r="B6" s="67">
         <v>13058093</v>
       </c>
-      <c r="C6" s="79">
+      <c r="C6" s="67">
         <v>5000000</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="78" t="s">
+      <c r="A7" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="79">
+      <c r="B7" s="67">
         <v>42360151</v>
       </c>
-      <c r="C7" s="79">
+      <c r="C7" s="67">
         <v>28514291.93</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" s="78" t="s">
+      <c r="A8" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="79">
+      <c r="B8" s="67">
         <v>2628307</v>
       </c>
-      <c r="C8" s="79">
+      <c r="C8" s="67">
         <v>2628307</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" s="78" t="s">
+      <c r="A9" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="79">
+      <c r="B9" s="67">
         <v>978421</v>
       </c>
-      <c r="C9" s="79">
+      <c r="C9" s="67">
         <v>978421</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" s="78" t="s">
+      <c r="A10" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="79">
+      <c r="B10" s="67">
         <v>32605795.710000001</v>
       </c>
-      <c r="C10" s="79">
+      <c r="C10" s="67">
         <v>23138107.899999999</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" s="78" t="s">
+      <c r="A11" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="79">
+      <c r="B11" s="67">
         <v>977007</v>
       </c>
-      <c r="C11" s="79">
+      <c r="C11" s="67">
         <v>977007</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12" s="78" t="s">
+      <c r="A12" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="79">
+      <c r="B12" s="67">
         <v>14767005</v>
       </c>
-      <c r="C12" s="79">
+      <c r="C12" s="67">
         <v>9659426.370000001</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13" s="78" t="s">
+      <c r="A13" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="79">
+      <c r="B13" s="67">
         <v>8059315</v>
       </c>
-      <c r="C13" s="79">
+      <c r="C13" s="67">
         <v>2304800</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A14" s="78" t="s">
+      <c r="A14" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="79">
+      <c r="B14" s="67">
         <v>978460</v>
       </c>
-      <c r="C14" s="79">
+      <c r="C14" s="67">
         <v>978460</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" s="78" t="s">
+      <c r="A15" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="79">
+      <c r="B15" s="67">
         <v>10173889</v>
       </c>
-      <c r="C15" s="79">
+      <c r="C15" s="67">
         <v>2138482.09</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A16" s="78" t="s">
+      <c r="A16" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="79">
+      <c r="B16" s="67">
         <v>16250065</v>
       </c>
-      <c r="C16" s="79">
+      <c r="C16" s="67">
         <v>6035928</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A17" s="78" t="s">
+      <c r="A17" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="79">
+      <c r="B17" s="67">
         <v>4070028</v>
       </c>
-      <c r="C17" s="79">
+      <c r="C17" s="67">
         <v>4064028</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" s="78" t="s">
+      <c r="A18" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="79">
+      <c r="B18" s="67">
         <v>6163501</v>
       </c>
-      <c r="C18" s="79">
+      <c r="C18" s="67">
         <v>1993648.65</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A19" s="78" t="s">
+      <c r="A19" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="79">
+      <c r="B19" s="67">
         <v>3105169</v>
       </c>
-      <c r="C19" s="79">
+      <c r="C19" s="67">
         <v>3625429</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A20" s="78" t="s">
+      <c r="A20" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="79">
+      <c r="B20" s="67">
         <v>6475917</v>
       </c>
-      <c r="C20" s="79">
+      <c r="C20" s="67">
         <v>6475917</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21" s="78" t="s">
+      <c r="A21" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="79">
+      <c r="B21" s="67">
         <v>39645631</v>
       </c>
-      <c r="C21" s="79">
+      <c r="C21" s="67">
         <v>37437345.109999999</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" s="78" t="s">
+      <c r="A22" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="79">
+      <c r="B22" s="67">
         <v>4926494</v>
       </c>
-      <c r="C22" s="79">
+      <c r="C22" s="67">
         <v>1560177.25</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A23" s="78" t="s">
+      <c r="A23" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="79">
+      <c r="B23" s="67">
         <v>1380115</v>
       </c>
-      <c r="C23" s="79">
+      <c r="C23" s="67">
         <v>1380115</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A24" s="78" t="s">
+      <c r="A24" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="79">
+      <c r="B24" s="67">
         <v>2944974</v>
       </c>
-      <c r="C24" s="79">
+      <c r="C24" s="67">
         <v>2944971</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A25" s="78" t="s">
+      <c r="A25" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="79">
+      <c r="B25" s="67">
         <v>10652930</v>
       </c>
-      <c r="C25" s="79">
+      <c r="C25" s="67">
         <v>10652720.32</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A26" s="78" t="s">
+      <c r="A26" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="79">
+      <c r="B26" s="67">
         <v>5788882</v>
       </c>
-      <c r="C26" s="79">
+      <c r="C26" s="67">
         <v>5446372</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A27" s="78" t="s">
+      <c r="A27" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="79">
+      <c r="B27" s="67">
         <v>9299420</v>
       </c>
-      <c r="C27" s="79">
+      <c r="C27" s="67">
         <v>9296766</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A28" s="78" t="s">
+      <c r="A28" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="79">
+      <c r="B28" s="67">
         <v>2730325</v>
       </c>
-      <c r="C28" s="79">
+      <c r="C28" s="67">
         <v>2730325</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A29" s="78" t="s">
+      <c r="A29" s="66" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="79">
+      <c r="B29" s="67">
         <v>4692095</v>
       </c>
-      <c r="C29" s="79">
+      <c r="C29" s="67">
         <v>4692089.46</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A30" s="78" t="s">
+      <c r="A30" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="79">
+      <c r="B30" s="67">
         <v>1653213</v>
       </c>
-      <c r="C30" s="79">
+      <c r="C30" s="67">
         <v>1652677</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A31" s="78" t="s">
+      <c r="A31" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="B31" s="79">
+      <c r="B31" s="67">
         <v>3301114</v>
       </c>
-      <c r="C31" s="79">
+      <c r="C31" s="67">
         <v>3301114</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A32" s="78" t="s">
+      <c r="A32" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="79">
+      <c r="B32" s="67">
         <v>22551603</v>
       </c>
-      <c r="C32" s="79">
+      <c r="C32" s="67">
         <v>21778540</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A33" s="78" t="s">
+      <c r="A33" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="79">
+      <c r="B33" s="67">
         <v>6554186</v>
       </c>
-      <c r="C33" s="79">
+      <c r="C33" s="67">
         <v>6554186</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A34" s="78" t="s">
+      <c r="A34" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="B34" s="79">
+      <c r="B34" s="67">
         <v>5492219</v>
       </c>
-      <c r="C34" s="79">
+      <c r="C34" s="67">
         <v>4283508</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A35" s="78" t="s">
+      <c r="A35" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="79">
+      <c r="B35" s="67">
         <v>8638087</v>
       </c>
-      <c r="C35" s="79">
+      <c r="C35" s="67">
         <v>8542014.6500000004</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A36" s="78" t="s">
+      <c r="A36" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="B36" s="79">
+      <c r="B36" s="67">
         <v>332487485.71000004</v>
       </c>
-      <c r="C36" s="79">
+      <c r="C36" s="67">
         <v>254062125.53000003</v>
       </c>
     </row>
@@ -2594,10 +2625,10 @@
   <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C37" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2613,1526 +2644,1527 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="58.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="33" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="48" customFormat="1" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:9" s="43" customFormat="1" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="16">
+        <v>11894913</v>
+      </c>
+      <c r="F2" s="42">
+        <v>44770</v>
+      </c>
+      <c r="G2" s="44">
+        <v>11782773</v>
+      </c>
+      <c r="H2" s="39" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="13">
+        <v>7900000</v>
+      </c>
+      <c r="F3" s="54">
+        <v>44481</v>
+      </c>
+      <c r="G3" s="56">
+        <f>6949908+457162+74808+37404</f>
+        <v>7519282</v>
+      </c>
+      <c r="H3" s="36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="17" t="s">
+      <c r="B4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="18">
-        <v>11894913</v>
-      </c>
-      <c r="F2" s="47">
-        <v>44770</v>
-      </c>
-      <c r="G2" s="49">
-        <v>11782773</v>
-      </c>
-      <c r="H2" s="44" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="11" t="s">
+      <c r="E4" s="12">
+        <v>10258000</v>
+      </c>
+      <c r="F4" s="17">
+        <v>44638</v>
+      </c>
+      <c r="G4" s="83">
+        <v>6027030.7999999998</v>
+      </c>
+      <c r="H4" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="36"/>
+    </row>
+    <row r="5" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="13">
+        <v>1144242</v>
+      </c>
+      <c r="F5" s="54">
+        <v>44418</v>
+      </c>
+      <c r="G5" s="84">
+        <v>1144242</v>
+      </c>
+      <c r="H5" s="62" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="13">
-        <v>10258000</v>
-      </c>
-      <c r="F3" s="19">
-        <v>44638</v>
-      </c>
-      <c r="G3" s="71">
-        <v>6027030.7999999998</v>
-      </c>
-      <c r="H3" s="41" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="52" t="s">
+      <c r="B6" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="9" t="s">
+      <c r="C6" s="46"/>
+      <c r="D6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E6" s="12">
         <v>1576793</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F6" s="81">
         <v>44851</v>
       </c>
-      <c r="G4" s="72">
+      <c r="G6" s="77">
         <v>92497</v>
       </c>
-      <c r="H4" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="41"/>
-    </row>
-    <row r="5" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="52" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="43">
-        <v>8058093</v>
-      </c>
-      <c r="F5" s="19"/>
-      <c r="H5" s="73" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="37">
-        <v>29107860</v>
-      </c>
-      <c r="F6" s="57">
-        <v>44782</v>
-      </c>
-      <c r="G6" s="68">
-        <v>15329692.93</v>
-      </c>
-      <c r="H6" s="53" t="s">
+      <c r="H6" s="47" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="36">
-        <v>9197974</v>
-      </c>
-      <c r="F7" s="58">
-        <v>44778</v>
-      </c>
-      <c r="G7" s="51">
-        <v>224976</v>
-      </c>
-      <c r="H7" s="41" t="s">
+      <c r="A7" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="13">
+        <v>1303508</v>
+      </c>
+      <c r="F7" s="55">
+        <v>44502</v>
+      </c>
+      <c r="G7" s="84">
+        <v>1303508</v>
+      </c>
+      <c r="H7" s="36" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="11" t="s">
-        <v>83</v>
+      <c r="A8" s="10" t="s">
+        <v>96</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="52" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="3">
-        <v>8407821.7100000009</v>
-      </c>
-      <c r="F8" s="4">
-        <v>44643</v>
-      </c>
-      <c r="G8" s="3">
-        <v>8182845.71</v>
+        <v>56</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="14">
+        <v>5507618</v>
+      </c>
+      <c r="F8" s="55">
+        <v>44489</v>
+      </c>
+      <c r="G8" s="57">
+        <f>196992+5230626</f>
+        <v>5427618</v>
       </c>
       <c r="H8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="11" t="s">
-        <v>84</v>
+      <c r="A9" s="10" t="s">
+        <v>97</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="14">
+        <v>978421</v>
+      </c>
+      <c r="F9" s="55">
+        <v>44491</v>
+      </c>
+      <c r="G9" s="56">
+        <f>292108+686313</f>
+        <v>978421</v>
+      </c>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="76">
+        <v>9197974</v>
+      </c>
+      <c r="F10" s="51">
+        <v>44778</v>
+      </c>
+      <c r="G10" s="86">
+        <v>224976</v>
+      </c>
+      <c r="H10" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="45" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="3">
+        <v>8407821.7100000009</v>
+      </c>
+      <c r="F11" s="4">
+        <v>44643</v>
+      </c>
+      <c r="G11" s="3">
+        <v>8182845.71</v>
+      </c>
+      <c r="H11" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="34"/>
+    </row>
+    <row r="12" spans="1:9" ht="34.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="14">
+        <v>15000000</v>
+      </c>
+      <c r="F12" s="55">
+        <v>44462</v>
+      </c>
+      <c r="G12" s="56">
+        <f>14600000+85612.5+44673.69</f>
+        <v>14730286.189999999</v>
+      </c>
+      <c r="H12" s="41" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="34.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9" t="s">
+      <c r="C13" s="7"/>
+      <c r="D13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E13" s="3">
         <v>12555809</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F13" s="4">
         <v>44638</v>
       </c>
-      <c r="G9" s="45">
+      <c r="G13" s="40">
         <f>6844818+349596+331058</f>
         <v>7525472</v>
       </c>
-      <c r="H9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="3">
-        <v>4100000</v>
-      </c>
-      <c r="F10" s="59"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="I10" s="50" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="55">
-        <v>8035407</v>
-      </c>
-      <c r="F11" s="59"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" s="38"/>
-    </row>
-    <row r="12" spans="1:9" ht="34.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="3">
-        <v>3000000</v>
-      </c>
-      <c r="F12" s="4">
-        <v>44551</v>
-      </c>
-      <c r="G12" s="3">
-        <v>1686683</v>
-      </c>
-      <c r="H12" s="46" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="34.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="3">
-        <v>8943548</v>
-      </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="69" t="s">
+      <c r="H13" s="60" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="11" t="s">
-        <v>88</v>
+      <c r="A14" s="10" t="s">
+        <v>82</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="3">
-        <v>542235</v>
-      </c>
-      <c r="F14" s="4">
-        <v>44551</v>
-      </c>
-      <c r="G14" s="3">
-        <v>542235</v>
+        <v>24</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="14">
+        <v>2211196</v>
+      </c>
+      <c r="F14" s="55">
+        <v>44462</v>
+      </c>
+      <c r="G14" s="56">
+        <f>1923741+80488+18469+86237+12446+12573.37</f>
+        <v>2133954.37</v>
       </c>
       <c r="H14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="11" t="s">
-        <v>88</v>
+      <c r="A15" s="10" t="s">
+        <v>83</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="3">
-        <v>4128053</v>
-      </c>
-      <c r="F15" s="4"/>
+        <v>4100000</v>
+      </c>
+      <c r="F15" s="52"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="70" t="s">
+      <c r="H15" s="61" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="11" t="s">
-        <v>89</v>
+      <c r="A16" s="10" t="s">
+        <v>83</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="3">
-        <v>2975917</v>
-      </c>
-      <c r="F16" s="4">
-        <v>44685</v>
-      </c>
-      <c r="G16" s="3">
-        <v>2975917</v>
+        <v>26</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="14">
+        <v>3959315</v>
+      </c>
+      <c r="F16" s="55">
+        <v>44511</v>
+      </c>
+      <c r="G16" s="56">
+        <f>2000000+107400+197400</f>
+        <v>2304800</v>
       </c>
       <c r="H16" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="11" t="s">
-        <v>90</v>
+      <c r="A17" t="s">
+        <v>105</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="14">
-        <v>23433350</v>
-      </c>
-      <c r="F17" s="60">
-        <v>44643</v>
-      </c>
-      <c r="G17" s="3">
-        <v>23433350</v>
+        <v>59</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="78">
+        <v>977007</v>
+      </c>
+      <c r="F17" s="55">
+        <v>44468</v>
+      </c>
+      <c r="G17" s="56">
+        <v>977007</v>
       </c>
       <c r="H17" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="11" t="s">
-        <v>90</v>
+      <c r="A18" s="10" t="s">
+        <v>98</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="78">
+        <v>978460</v>
+      </c>
+      <c r="F18" s="55">
+        <v>44489</v>
+      </c>
+      <c r="G18" s="56">
+        <v>978460</v>
+      </c>
+      <c r="H18" s="50" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="49">
+        <v>8035407</v>
+      </c>
+      <c r="F19" s="52"/>
+      <c r="G19" s="3"/>
+      <c r="H19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="28.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="78">
+        <v>2138482</v>
+      </c>
+      <c r="F20" s="55">
+        <v>44496</v>
+      </c>
+      <c r="G20" s="56">
+        <f>1686666.67+451815.42</f>
+        <v>2138482.09</v>
+      </c>
+      <c r="H20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="40.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="F21" s="4">
+        <v>44551</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1686683</v>
+      </c>
+      <c r="H21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="34.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="3">
+        <v>8943548</v>
+      </c>
+      <c r="F22" s="4"/>
+      <c r="G22" s="3"/>
+      <c r="H22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="14">
+        <v>4306517</v>
+      </c>
+      <c r="F23" s="55">
+        <v>44432</v>
+      </c>
+      <c r="G23" s="56">
+        <f>500000+2306517+200000+26944.5+15783.5+1300000</f>
+        <v>4349245</v>
+      </c>
+      <c r="H23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="14">
+        <v>4070028</v>
+      </c>
+      <c r="F24" s="55">
+        <v>44439</v>
+      </c>
+      <c r="G24" s="56">
+        <f>3982627+81401</f>
+        <v>4064028</v>
+      </c>
+      <c r="H24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="45.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="78">
+        <v>3105169</v>
+      </c>
+      <c r="F25" s="55">
+        <v>44511</v>
+      </c>
+      <c r="G25" s="56">
+        <f>124207+3377016+124206</f>
+        <v>3625429</v>
+      </c>
+      <c r="H25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="45.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="7"/>
+      <c r="D26" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="75">
+        <v>542235</v>
+      </c>
+      <c r="F26" s="4">
+        <v>44551</v>
+      </c>
+      <c r="G26" s="3">
+        <v>542235</v>
+      </c>
+      <c r="H26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="40.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="75">
+        <v>4128053</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="3"/>
+      <c r="H27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="78">
+        <v>1493213</v>
+      </c>
+      <c r="F28" s="55">
+        <v>44505</v>
+      </c>
+      <c r="G28" s="56">
+        <f>779887.65+589325+70000+12201</f>
+        <v>1451413.65</v>
+      </c>
+      <c r="H28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="3">
+        <v>2975917</v>
+      </c>
+      <c r="F29" s="4">
+        <v>44685</v>
+      </c>
+      <c r="G29" s="3">
+        <v>2975917</v>
+      </c>
+      <c r="H29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" s="14">
+        <v>3500000</v>
+      </c>
+      <c r="F30" s="55">
+        <v>44462</v>
+      </c>
+      <c r="G30" s="58">
+        <v>3500000</v>
+      </c>
+      <c r="H30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C31" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D31" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="40">
+      <c r="E31" s="3">
+        <v>23433350</v>
+      </c>
+      <c r="F31" s="53">
+        <v>44643</v>
+      </c>
+      <c r="G31" s="3">
+        <v>23433350</v>
+      </c>
+      <c r="H31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" s="68" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="68" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="38">
         <v>6216901</v>
       </c>
-      <c r="F18" s="60">
+      <c r="F32" s="87">
         <v>44805</v>
       </c>
-      <c r="G18" s="54">
+      <c r="G32" s="88">
         <v>3581632</v>
       </c>
-      <c r="H18" s="56" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="B19" s="6" t="s">
+      <c r="H32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="10"/>
+      <c r="D33" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" s="14">
+        <v>9995380</v>
+      </c>
+      <c r="F33" s="55">
+        <v>44484</v>
+      </c>
+      <c r="G33" s="57">
+        <f>5124130+4871251+60661.74+366320.37</f>
+        <v>10422363.109999999</v>
+      </c>
+      <c r="H33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9" t="s">
+      <c r="C34" s="68"/>
+      <c r="D34" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E34" s="3">
         <v>2180890</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F34" s="4">
         <v>44665</v>
       </c>
-      <c r="G19" s="45">
+      <c r="G34" s="40">
         <f>942269+586829</f>
         <v>1529098</v>
       </c>
-      <c r="H19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="28.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B20" s="6" t="s">
+      <c r="H34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="10"/>
+      <c r="D35" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E35" s="14">
+        <v>2745604</v>
+      </c>
+      <c r="F35" s="55">
+        <v>44547</v>
+      </c>
+      <c r="G35" s="56">
+        <v>31079.25</v>
+      </c>
+      <c r="H35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="68" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="3">
+        <v>5763000</v>
+      </c>
+      <c r="F36" s="4">
+        <v>44699</v>
+      </c>
+      <c r="G36" s="3">
+        <v>5760333</v>
+      </c>
+      <c r="H36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="10"/>
+      <c r="D37" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E37" s="14">
+        <v>3536420</v>
+      </c>
+      <c r="F37" s="55">
+        <v>44533</v>
+      </c>
+      <c r="G37" s="56">
+        <f>1124355+2412078</f>
+        <v>3536433</v>
+      </c>
+      <c r="H37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A38" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="10"/>
+      <c r="D38" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E38" s="14">
+        <v>1380115</v>
+      </c>
+      <c r="F38" s="55">
+        <v>44484</v>
+      </c>
+      <c r="G38" s="56">
+        <v>1380115</v>
+      </c>
+      <c r="H38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="74" t="s">
+      <c r="C39" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D39" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E39" s="3">
         <v>1977284</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F39" s="4">
         <v>44631</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G39" s="3">
         <v>1977284</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H39" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="40.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="B21" s="6" t="s">
+    <row r="40" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" s="10"/>
+      <c r="D40" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E40" s="14">
+        <v>967690</v>
+      </c>
+      <c r="F40" s="55">
+        <v>44468</v>
+      </c>
+      <c r="G40" s="56">
+        <f>252647+715040</f>
+        <v>967687</v>
+      </c>
+      <c r="H40" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C41" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D41" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E41" s="3">
         <v>5552930</v>
       </c>
-      <c r="F21" s="39">
+      <c r="F41" s="35">
         <v>44754</v>
       </c>
-      <c r="G21" s="45">
+      <c r="G41" s="40">
         <f>2784017.52+2375672.8+152280+240750</f>
         <v>5552720.3200000003</v>
       </c>
-      <c r="H21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="34.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="B22" s="6" t="s">
+      <c r="H41" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" s="10"/>
+      <c r="D42" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E42" s="14">
+        <v>5100000</v>
+      </c>
+      <c r="F42" s="55">
+        <v>44502</v>
+      </c>
+      <c r="G42" s="56">
+        <f>2275285+2824715</f>
+        <v>5100000</v>
+      </c>
+      <c r="H42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A43" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C43" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D43" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E43" s="3">
         <v>2800000</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F43" s="4">
         <v>44685</v>
       </c>
-      <c r="G22" s="75">
+      <c r="G43" s="63">
         <v>2584985</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H43" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="9" t="s">
+    <row r="44" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" s="10"/>
+      <c r="D44" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E44" s="14">
+        <v>2988882</v>
+      </c>
+      <c r="F44" s="55">
+        <v>44491</v>
+      </c>
+      <c r="G44" s="56">
+        <f>963663+970391+757400+58062+17250+29031+65590</f>
+        <v>2861387</v>
+      </c>
+      <c r="H44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" s="10"/>
+      <c r="D45" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E45" s="14">
+        <v>2730325</v>
+      </c>
+      <c r="F45" s="55">
+        <v>44510</v>
+      </c>
+      <c r="G45" s="56">
+        <f>1365162.5+1365162.5</f>
+        <v>2730325</v>
+      </c>
+      <c r="H45" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A46" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" s="68"/>
+      <c r="D46" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="3">
-        <v>5763000</v>
-      </c>
-      <c r="F23" s="4">
-        <v>44699</v>
-      </c>
-      <c r="G23" s="3">
-        <v>5760333</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="E46" s="3">
+        <v>4692095</v>
+      </c>
+      <c r="F46" s="4">
+        <v>44692</v>
+      </c>
+      <c r="G46" s="3">
+        <v>4692089.46</v>
+      </c>
+      <c r="H46" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9" t="s">
+    <row r="47" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" s="68"/>
+      <c r="D47" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="3">
-        <v>4692095</v>
-      </c>
-      <c r="F24" s="4">
-        <v>44692</v>
-      </c>
-      <c r="G24" s="3">
-        <v>4692089.46</v>
-      </c>
-      <c r="H24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="45.7" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="14">
+      <c r="E47" s="3">
         <v>1653213</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F47" s="4">
         <v>44726</v>
       </c>
-      <c r="G25" s="45">
+      <c r="G47" s="40">
         <f>752120+900557</f>
         <v>1652677</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H47" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="45.7" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" s="6" t="s">
+    <row r="48" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B48" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="9" t="s">
+      <c r="C48" s="68"/>
+      <c r="D48" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="40">
+      <c r="E48" s="74">
         <v>3301114</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F48" s="4">
         <v>44775</v>
       </c>
-      <c r="G26" s="54">
+      <c r="G48" s="48">
         <v>3301114</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H48" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="40.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="7">
-        <v>4899111</v>
-      </c>
-      <c r="F27" s="4">
-        <v>44665</v>
-      </c>
-      <c r="G27" s="3">
-        <v>4899111</v>
-      </c>
-      <c r="H27" t="s">
+    <row r="49" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49" s="69" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="D49" s="72" t="s">
+        <v>14</v>
+      </c>
+      <c r="E49" s="74">
+        <v>8058093</v>
+      </c>
+      <c r="F49" s="4"/>
+      <c r="G49" s="85"/>
+      <c r="H49" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="7">
-        <v>10900000</v>
-      </c>
-      <c r="F28" s="4">
-        <v>44747</v>
-      </c>
-      <c r="G28" s="42">
-        <v>10126937</v>
-      </c>
-      <c r="H28" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="3">
-        <v>3000000</v>
-      </c>
-      <c r="F29" s="4">
-        <v>44617</v>
-      </c>
-      <c r="G29" s="3">
-        <v>3000000</v>
-      </c>
-      <c r="H29" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="3">
-        <v>1208710</v>
-      </c>
-      <c r="F30" s="4"/>
-      <c r="G30" s="3"/>
-      <c r="H30" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="3">
-        <v>6717249</v>
-      </c>
-      <c r="F31" s="4">
-        <v>44719</v>
-      </c>
-      <c r="G31" s="76">
-        <v>6621177</v>
-      </c>
-      <c r="H31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="5" t="s">
+    <row r="50" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" s="10"/>
+      <c r="D50" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E32" s="15">
-        <v>7900000</v>
-      </c>
-      <c r="F32" s="61">
-        <v>44481</v>
-      </c>
-      <c r="G32" s="63">
-        <f>6949908+457162+74808+37404</f>
-        <v>7519282</v>
-      </c>
-      <c r="H32" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="11"/>
-      <c r="D33" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E33" s="16">
-        <v>1144242</v>
-      </c>
-      <c r="F33" s="62">
-        <v>44418</v>
-      </c>
-      <c r="G33" s="64">
-        <v>1144242</v>
-      </c>
-      <c r="H33" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E34" s="16">
-        <v>5507618</v>
-      </c>
-      <c r="F34" s="62">
-        <v>44489</v>
-      </c>
-      <c r="G34" s="65">
-        <f>196992+5230626</f>
-        <v>5427618</v>
-      </c>
-      <c r="H34" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E35" s="16">
-        <v>1303508</v>
-      </c>
-      <c r="F35" s="62">
+      <c r="E50" s="14">
+        <v>5000000</v>
+      </c>
+      <c r="F50" s="55">
         <v>44502</v>
       </c>
-      <c r="G35" s="64">
-        <v>1303508</v>
-      </c>
-      <c r="H35" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E36" s="16">
-        <v>5000000</v>
-      </c>
-      <c r="F36" s="62">
-        <v>44502</v>
-      </c>
-      <c r="G36" s="64">
+      <c r="G50" s="56">
         <f>4000000+700000+300000</f>
         <v>5000000</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H50" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B37" s="6" t="s">
+    <row r="51" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>103</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51" s="68"/>
+      <c r="D51" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="79">
+        <v>4899111</v>
+      </c>
+      <c r="F51" s="4">
+        <v>44665</v>
+      </c>
+      <c r="G51" s="3">
+        <v>4899111</v>
+      </c>
+      <c r="H51" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>103</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C52" s="68"/>
+      <c r="D52" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" s="79">
+        <v>10900000</v>
+      </c>
+      <c r="F52" s="4">
+        <v>44747</v>
+      </c>
+      <c r="G52" s="37">
+        <v>10126937</v>
+      </c>
+      <c r="H52" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>103</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C53" s="10"/>
+      <c r="D53" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E53" s="14">
+        <v>6752492</v>
+      </c>
+      <c r="F53" s="55">
+        <v>44439</v>
+      </c>
+      <c r="G53" s="56">
+        <v>6752492</v>
+      </c>
+      <c r="H53" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A54" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C54" s="68"/>
+      <c r="D54" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="F54" s="4">
+        <v>44617</v>
+      </c>
+      <c r="G54" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="H54" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A55" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C55" s="10"/>
+      <c r="D55" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E55" s="14">
+        <v>3554186</v>
+      </c>
+      <c r="F55" s="55">
+        <v>44418</v>
+      </c>
+      <c r="G55" s="56">
+        <f>3554186</f>
+        <v>3554186</v>
+      </c>
+      <c r="H55" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>104</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C56" s="68" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="3">
+        <v>1208710</v>
+      </c>
+      <c r="F56" s="4"/>
+      <c r="G56" s="3"/>
+      <c r="H56" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>104</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C57" s="10"/>
+      <c r="D57" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E57" s="14">
+        <v>4283509</v>
+      </c>
+      <c r="F57" s="55">
+        <v>44505</v>
+      </c>
+      <c r="G57" s="56">
+        <f>1043077+3240431</f>
+        <v>4283508</v>
+      </c>
+      <c r="H57" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A58" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C58" s="68"/>
+      <c r="D58" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="3">
+        <v>6717249</v>
+      </c>
+      <c r="F58" s="4">
+        <v>44719</v>
+      </c>
+      <c r="G58" s="64">
+        <v>6621177</v>
+      </c>
+      <c r="H58" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A59" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C59" s="10"/>
+      <c r="D59" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E59" s="14">
+        <v>1920838</v>
+      </c>
+      <c r="F59" s="55">
+        <v>44489</v>
+      </c>
+      <c r="G59" s="57">
+        <f>637595+472476+810766.65</f>
+        <v>1920837.65</v>
+      </c>
+      <c r="H59" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>106</v>
+      </c>
+      <c r="B60" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="C37" s="11"/>
-      <c r="D37" s="5" t="s">
+      <c r="C60" s="70"/>
+      <c r="D60" s="72" t="s">
+        <v>14</v>
+      </c>
+      <c r="E60" s="73">
+        <v>29107860</v>
+      </c>
+      <c r="F60" s="80">
+        <v>44782</v>
+      </c>
+      <c r="G60" s="82">
+        <v>15329692.93</v>
+      </c>
+      <c r="H60" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>106</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C61" s="10"/>
+      <c r="D61" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E37" s="16">
+      <c r="E61" s="14">
         <v>13252291</v>
       </c>
-      <c r="F37" s="62">
+      <c r="F61" s="55">
         <v>44474</v>
       </c>
-      <c r="G37" s="64">
+      <c r="G61" s="56">
         <f>3009307+8507891+1667401</f>
         <v>13184599</v>
       </c>
-      <c r="H37" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C38" s="11"/>
-      <c r="D38" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E38" s="16">
-        <v>2628307</v>
-      </c>
-      <c r="F38" s="62">
-        <v>44487</v>
-      </c>
-      <c r="G38" s="65">
-        <v>2628307</v>
-      </c>
-      <c r="H38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C39" s="11"/>
-      <c r="D39" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E39" s="16">
-        <v>978421</v>
-      </c>
-      <c r="F39" s="62">
-        <v>44491</v>
-      </c>
-      <c r="G39" s="64">
-        <f>292108+686313</f>
-        <v>978421</v>
-      </c>
-      <c r="H39" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C40" s="11"/>
-      <c r="D40" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E40" s="16">
-        <v>15000000</v>
-      </c>
-      <c r="F40" s="62">
-        <v>44462</v>
-      </c>
-      <c r="G40" s="64">
-        <f>14600000+85612.5+44673.69</f>
-        <v>14730286.189999999</v>
-      </c>
-      <c r="H40" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C41" s="11"/>
-      <c r="D41" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E41" s="16">
-        <v>977007</v>
-      </c>
-      <c r="F41" s="62">
-        <v>44468</v>
-      </c>
-      <c r="G41" s="64">
-        <v>977007</v>
-      </c>
-      <c r="H41" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C42" s="11"/>
-      <c r="D42" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E42" s="16">
-        <v>2211196</v>
-      </c>
-      <c r="F42" s="62">
-        <v>44462</v>
-      </c>
-      <c r="G42" s="64">
-        <f>1923741+80488+18469+86237+12446+12573.37</f>
-        <v>2133954.37</v>
-      </c>
-      <c r="H42" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C43" s="11"/>
-      <c r="D43" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E43" s="16">
-        <v>3959315</v>
-      </c>
-      <c r="F43" s="62">
-        <v>44511</v>
-      </c>
-      <c r="G43" s="64">
-        <f>2000000+107400+197400</f>
-        <v>2304800</v>
-      </c>
-      <c r="H43" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C44" s="11"/>
-      <c r="D44" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E44" s="16">
-        <v>978460</v>
-      </c>
-      <c r="F44" s="62">
-        <v>44489</v>
-      </c>
-      <c r="G44" s="64">
-        <v>978460</v>
-      </c>
-      <c r="H44" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C45" s="11"/>
-      <c r="D45" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E45" s="16">
-        <v>2138482</v>
-      </c>
-      <c r="F45" s="62">
-        <v>44496</v>
-      </c>
-      <c r="G45" s="64">
-        <f>1686666.67+451815.42</f>
-        <v>2138482.09</v>
-      </c>
-      <c r="H45" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C46" s="11"/>
-      <c r="D46" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E46" s="16">
-        <v>4306517</v>
-      </c>
-      <c r="F46" s="62">
-        <v>44432</v>
-      </c>
-      <c r="G46" s="64">
-        <f>500000+2306517+200000+26944.5+15783.5+1300000</f>
-        <v>4349245</v>
-      </c>
-      <c r="H46" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C47" s="11"/>
-      <c r="D47" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E47" s="16">
-        <v>4070028</v>
-      </c>
-      <c r="F47" s="62">
-        <v>44439</v>
-      </c>
-      <c r="G47" s="64">
-        <f>3982627+81401</f>
-        <v>4064028</v>
-      </c>
-      <c r="H47" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C48" s="11"/>
-      <c r="D48" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E48" s="16">
-        <v>1493213</v>
-      </c>
-      <c r="F48" s="62">
-        <v>44505</v>
-      </c>
-      <c r="G48" s="64">
-        <f>779887.65+589325+70000+12201</f>
-        <v>1451413.65</v>
-      </c>
-      <c r="H48" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C49" s="11"/>
-      <c r="D49" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E49" s="16">
-        <v>3105169</v>
-      </c>
-      <c r="F49" s="62">
-        <v>44511</v>
-      </c>
-      <c r="G49" s="64">
-        <f>124207+3377016+124206</f>
-        <v>3625429</v>
-      </c>
-      <c r="H49" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C50" s="11"/>
-      <c r="D50" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E50" s="16">
-        <v>3500000</v>
-      </c>
-      <c r="F50" s="62">
-        <v>44462</v>
-      </c>
-      <c r="G50" s="66">
-        <v>3500000</v>
-      </c>
-      <c r="H50" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C51" s="11"/>
-      <c r="D51" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E51" s="16">
-        <v>9995380</v>
-      </c>
-      <c r="F51" s="62">
-        <v>44484</v>
-      </c>
-      <c r="G51" s="65">
-        <f>5124130+4871251+60661.74+366320.37</f>
-        <v>10422363.109999999</v>
-      </c>
-      <c r="H51" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C52" s="11"/>
-      <c r="D52" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E52" s="16">
-        <v>2745604</v>
-      </c>
-      <c r="F52" s="62">
-        <v>44547</v>
-      </c>
-      <c r="G52" s="64">
-        <v>31079.25</v>
-      </c>
-      <c r="H52" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C53" s="11"/>
-      <c r="D53" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E53" s="16">
-        <v>1380115</v>
-      </c>
-      <c r="F53" s="62">
-        <v>44484</v>
-      </c>
-      <c r="G53" s="64">
-        <v>1380115</v>
-      </c>
-      <c r="H53" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C54" s="11"/>
-      <c r="D54" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E54" s="16">
-        <v>967690</v>
-      </c>
-      <c r="F54" s="62">
-        <v>44468</v>
-      </c>
-      <c r="G54" s="64">
-        <f>252647+715040</f>
-        <v>967687</v>
-      </c>
-      <c r="H54" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C55" s="11"/>
-      <c r="D55" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E55" s="16">
-        <v>5100000</v>
-      </c>
-      <c r="F55" s="62">
-        <v>44502</v>
-      </c>
-      <c r="G55" s="64">
-        <f>2275285+2824715</f>
-        <v>5100000</v>
-      </c>
-      <c r="H55" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C56" s="11"/>
-      <c r="D56" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E56" s="16">
-        <v>2988882</v>
-      </c>
-      <c r="F56" s="62">
-        <v>44491</v>
-      </c>
-      <c r="G56" s="64">
-        <f>963663+970391+757400+58062+17250+29031+65590</f>
-        <v>2861387</v>
-      </c>
-      <c r="H56" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C57" s="11"/>
-      <c r="D57" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E57" s="16">
-        <v>3536420</v>
-      </c>
-      <c r="F57" s="62">
-        <v>44533</v>
-      </c>
-      <c r="G57" s="64">
-        <f>1124355+2412078</f>
-        <v>3536433</v>
-      </c>
-      <c r="H57" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B58" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C58" s="11"/>
-      <c r="D58" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E58" s="16">
-        <v>2730325</v>
-      </c>
-      <c r="F58" s="62">
-        <v>44510</v>
-      </c>
-      <c r="G58" s="64">
-        <f>1365162.5+1365162.5</f>
-        <v>2730325</v>
-      </c>
-      <c r="H58" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C59" s="11"/>
-      <c r="D59" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E59" s="16">
-        <v>6752492</v>
-      </c>
-      <c r="F59" s="62">
-        <v>44439</v>
-      </c>
-      <c r="G59" s="64">
-        <v>6752492</v>
-      </c>
-      <c r="H59" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A60" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C60" s="11"/>
-      <c r="D60" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E60" s="16">
-        <v>3554186</v>
-      </c>
-      <c r="F60" s="62">
-        <v>44418</v>
-      </c>
-      <c r="G60" s="64">
-        <f>3554186</f>
-        <v>3554186</v>
-      </c>
-      <c r="H60" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A61" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C61" s="11"/>
-      <c r="D61" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E61" s="16">
-        <v>4283509</v>
-      </c>
-      <c r="F61" s="62">
-        <v>44505</v>
-      </c>
-      <c r="G61" s="64">
-        <f>1043077+3240431</f>
-        <v>4283508</v>
-      </c>
       <c r="H61" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="11" t="s">
-        <v>99</v>
+      <c r="A62" t="s">
+        <v>107</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C62" s="11"/>
+        <v>57</v>
+      </c>
+      <c r="C62" s="10"/>
       <c r="D62" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E62" s="16">
-        <v>1920838</v>
-      </c>
-      <c r="F62" s="62">
-        <v>44489</v>
-      </c>
-      <c r="G62" s="65">
-        <f>637595+472476+810766.65</f>
-        <v>1920837.65</v>
+      <c r="E62" s="14">
+        <v>2628307</v>
+      </c>
+      <c r="F62" s="55">
+        <v>44487</v>
+      </c>
+      <c r="G62" s="57">
+        <v>2628307</v>
       </c>
       <c r="H62" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G63" s="41"/>
+      <c r="G63" s="36"/>
     </row>
   </sheetData>
   <protectedRanges>
@@ -4187,46 +4219,46 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="20"/>
+      <c r="B2" s="18"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="19"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="26"/>
+      <c r="B4" s="24"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="22"/>
+      <c r="B5" s="20"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="24"/>
+      <c r="B6" s="22"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="23"/>
+      <c r="B7" s="21"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="25"/>
+      <c r="B8" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4238,21 +4270,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001F87334A6AC30D4EA6021977FA7E2445" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="13eff9136b4917bb459ad9c1db870f6d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b370a6fa-a798-42e0-969d-19c284d8683f" xmlns:ns3="62ca1376-8bea-4949-825e-fec085c3924e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="60e7197df19c7150b1ba0c3bfe00adf4" ns2:_="" ns3:_="">
     <xsd:import namespace="b370a6fa-a798-42e0-969d-19c284d8683f"/>
@@ -4469,15 +4492,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DDCF067-268F-4A3C-A288-B4575E68AABA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{752D7A7F-0D65-4907-85A4-76807BF1350E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4489,7 +4513,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D681DB6D-9136-4740-BD99-737079D2FCBE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4506,4 +4530,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DDCF067-268F-4A3C-A288-B4575E68AABA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Changes to adm_consolidate to cap coverage figures
</commit_message>
<xml_diff>
--- a/data/input/base_financing_cds.xlsx
+++ b/data/input/base_financing_cds.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
-  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg-my.sharepoint.com/personal/panlilioj_who_int/Documents/covid19_vaccination_analysis/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{26E979B5-FA10-4638-B812-BC8073066A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDD1422A-CFCF-4956-9672-D63CAB2CD968}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{26E979B5-FA10-4638-B812-BC8073066A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{811E209E-4D9A-416A-82DE-D29085A772AB}"/>
   <bookViews>
     <workbookView xWindow="28690" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{FD644F38-BFEB-4730-9E59-BCD9CF33A41F}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -365,97 +365,97 @@
     <t>ISO</t>
   </si>
   <si>
+    <t>AFG</t>
+  </si>
+  <si>
+    <t>BFA</t>
+  </si>
+  <si>
+    <t>CAF</t>
+  </si>
+  <si>
+    <t>TCD</t>
+  </si>
+  <si>
+    <t>ETH</t>
+  </si>
+  <si>
+    <t>GHA</t>
+  </si>
+  <si>
+    <t>GIN</t>
+  </si>
+  <si>
+    <t>HTI</t>
+  </si>
+  <si>
+    <t>KEN</t>
+  </si>
+  <si>
+    <t>MWI</t>
+  </si>
+  <si>
+    <t>NER</t>
+  </si>
+  <si>
+    <t>NGA</t>
+  </si>
+  <si>
+    <t>PNG</t>
+  </si>
+  <si>
+    <t>SLE</t>
+  </si>
+  <si>
+    <t>SOM</t>
+  </si>
+  <si>
+    <t>SSD</t>
+  </si>
+  <si>
+    <t>SDN</t>
+  </si>
+  <si>
+    <t>UGA</t>
+  </si>
+  <si>
+    <t>ZMB</t>
+  </si>
+  <si>
+    <t>CMR</t>
+  </si>
+  <si>
+    <t>DJI</t>
+  </si>
+  <si>
+    <t>GNB</t>
+  </si>
+  <si>
+    <t>MDG</t>
+  </si>
+  <si>
+    <t>MLI</t>
+  </si>
+  <si>
+    <t>SEN</t>
+  </si>
+  <si>
     <t>SYR</t>
   </si>
   <si>
-    <t>AFG</t>
-  </si>
-  <si>
-    <t>BFA</t>
-  </si>
-  <si>
-    <t>CAF</t>
-  </si>
-  <si>
-    <t>TCD</t>
+    <t>TZA</t>
+  </si>
+  <si>
+    <t>YEM</t>
+  </si>
+  <si>
+    <t>GMB</t>
   </si>
   <si>
     <t>COD</t>
   </si>
   <si>
-    <t>ETH</t>
-  </si>
-  <si>
-    <t>GHA</t>
-  </si>
-  <si>
-    <t>GIN</t>
-  </si>
-  <si>
-    <t>HTI</t>
-  </si>
-  <si>
-    <t>KEN</t>
-  </si>
-  <si>
-    <t>MWI</t>
-  </si>
-  <si>
-    <t>NER</t>
-  </si>
-  <si>
-    <t>NGA</t>
-  </si>
-  <si>
-    <t>PNG</t>
-  </si>
-  <si>
-    <t>SLE</t>
-  </si>
-  <si>
-    <t>SOM</t>
-  </si>
-  <si>
-    <t>SSD</t>
-  </si>
-  <si>
-    <t>SDN</t>
-  </si>
-  <si>
-    <t>TZA</t>
-  </si>
-  <si>
-    <t>UGA</t>
-  </si>
-  <si>
-    <t>YEM</t>
-  </si>
-  <si>
-    <t>ZMB</t>
-  </si>
-  <si>
-    <t>CMR</t>
-  </si>
-  <si>
     <t>CIV</t>
-  </si>
-  <si>
-    <t>DJI</t>
-  </si>
-  <si>
-    <t>GMB</t>
-  </si>
-  <si>
-    <t>GNB</t>
-  </si>
-  <si>
-    <t>MDG</t>
-  </si>
-  <si>
-    <t>MLI</t>
-  </si>
-  <si>
-    <t>SEN</t>
   </si>
 </sst>
 </file>
@@ -738,7 +738,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -755,9 +755,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -780,7 +777,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -819,13 +815,10 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="12" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="169" fontId="6" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -850,7 +843,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -862,9 +854,6 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="6" fillId="13" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -880,9 +869,6 @@
     <xf numFmtId="169" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -895,16 +881,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="13" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="40" fontId="0" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="40" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -912,6 +891,54 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="12" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="12" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="40% - Accent4 5" xfId="4" xr:uid="{BBE1C5CD-EB81-46A5-A1EB-6EEB64CB90EF}"/>
@@ -974,6 +1001,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1666,7 +1697,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C9206A13-E1F8-4BA4-9E83-D2C707B1EEF4}" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C9206A13-E1F8-4BA4-9E83-D2C707B1EEF4}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:C36" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
@@ -2189,7 +2220,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="65" t="s">
         <v>72</v>
       </c>
       <c r="B1" t="s">
@@ -2200,387 +2231,387 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="79">
+      <c r="B2" s="67">
         <v>19794913</v>
       </c>
-      <c r="C2" s="79">
+      <c r="C2" s="67">
         <v>19302055</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="79">
+      <c r="B3" s="67">
         <v>11402242</v>
       </c>
-      <c r="C3" s="79">
+      <c r="C3" s="67">
         <v>7171272.7999999998</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="79">
+      <c r="B4" s="67">
         <v>5507618</v>
       </c>
-      <c r="C4" s="79">
+      <c r="C4" s="67">
         <v>5427618</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="79">
+      <c r="B5" s="67">
         <v>2880301</v>
       </c>
-      <c r="C5" s="79">
+      <c r="C5" s="67">
         <v>1396005</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="79">
+      <c r="B6" s="67">
         <v>13058093</v>
       </c>
-      <c r="C6" s="79">
+      <c r="C6" s="67">
         <v>5000000</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="78" t="s">
+      <c r="A7" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="79">
+      <c r="B7" s="67">
         <v>42360151</v>
       </c>
-      <c r="C7" s="79">
+      <c r="C7" s="67">
         <v>28514291.93</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" s="78" t="s">
+      <c r="A8" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="79">
+      <c r="B8" s="67">
         <v>2628307</v>
       </c>
-      <c r="C8" s="79">
+      <c r="C8" s="67">
         <v>2628307</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" s="78" t="s">
+      <c r="A9" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="79">
+      <c r="B9" s="67">
         <v>978421</v>
       </c>
-      <c r="C9" s="79">
+      <c r="C9" s="67">
         <v>978421</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" s="78" t="s">
+      <c r="A10" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="79">
+      <c r="B10" s="67">
         <v>32605795.710000001</v>
       </c>
-      <c r="C10" s="79">
+      <c r="C10" s="67">
         <v>23138107.899999999</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" s="78" t="s">
+      <c r="A11" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="79">
+      <c r="B11" s="67">
         <v>977007</v>
       </c>
-      <c r="C11" s="79">
+      <c r="C11" s="67">
         <v>977007</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12" s="78" t="s">
+      <c r="A12" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="79">
+      <c r="B12" s="67">
         <v>14767005</v>
       </c>
-      <c r="C12" s="79">
+      <c r="C12" s="67">
         <v>9659426.370000001</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13" s="78" t="s">
+      <c r="A13" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="79">
+      <c r="B13" s="67">
         <v>8059315</v>
       </c>
-      <c r="C13" s="79">
+      <c r="C13" s="67">
         <v>2304800</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A14" s="78" t="s">
+      <c r="A14" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="79">
+      <c r="B14" s="67">
         <v>978460</v>
       </c>
-      <c r="C14" s="79">
+      <c r="C14" s="67">
         <v>978460</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" s="78" t="s">
+      <c r="A15" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="79">
+      <c r="B15" s="67">
         <v>10173889</v>
       </c>
-      <c r="C15" s="79">
+      <c r="C15" s="67">
         <v>2138482.09</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A16" s="78" t="s">
+      <c r="A16" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="79">
+      <c r="B16" s="67">
         <v>16250065</v>
       </c>
-      <c r="C16" s="79">
+      <c r="C16" s="67">
         <v>6035928</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A17" s="78" t="s">
+      <c r="A17" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="79">
+      <c r="B17" s="67">
         <v>4070028</v>
       </c>
-      <c r="C17" s="79">
+      <c r="C17" s="67">
         <v>4064028</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" s="78" t="s">
+      <c r="A18" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="79">
+      <c r="B18" s="67">
         <v>6163501</v>
       </c>
-      <c r="C18" s="79">
+      <c r="C18" s="67">
         <v>1993648.65</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A19" s="78" t="s">
+      <c r="A19" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="79">
+      <c r="B19" s="67">
         <v>3105169</v>
       </c>
-      <c r="C19" s="79">
+      <c r="C19" s="67">
         <v>3625429</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A20" s="78" t="s">
+      <c r="A20" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="79">
+      <c r="B20" s="67">
         <v>6475917</v>
       </c>
-      <c r="C20" s="79">
+      <c r="C20" s="67">
         <v>6475917</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21" s="78" t="s">
+      <c r="A21" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="79">
+      <c r="B21" s="67">
         <v>39645631</v>
       </c>
-      <c r="C21" s="79">
+      <c r="C21" s="67">
         <v>37437345.109999999</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" s="78" t="s">
+      <c r="A22" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="79">
+      <c r="B22" s="67">
         <v>4926494</v>
       </c>
-      <c r="C22" s="79">
+      <c r="C22" s="67">
         <v>1560177.25</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A23" s="78" t="s">
+      <c r="A23" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="79">
+      <c r="B23" s="67">
         <v>1380115</v>
       </c>
-      <c r="C23" s="79">
+      <c r="C23" s="67">
         <v>1380115</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A24" s="78" t="s">
+      <c r="A24" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="79">
+      <c r="B24" s="67">
         <v>2944974</v>
       </c>
-      <c r="C24" s="79">
+      <c r="C24" s="67">
         <v>2944971</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A25" s="78" t="s">
+      <c r="A25" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="79">
+      <c r="B25" s="67">
         <v>10652930</v>
       </c>
-      <c r="C25" s="79">
+      <c r="C25" s="67">
         <v>10652720.32</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A26" s="78" t="s">
+      <c r="A26" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="79">
+      <c r="B26" s="67">
         <v>5788882</v>
       </c>
-      <c r="C26" s="79">
+      <c r="C26" s="67">
         <v>5446372</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A27" s="78" t="s">
+      <c r="A27" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="79">
+      <c r="B27" s="67">
         <v>9299420</v>
       </c>
-      <c r="C27" s="79">
+      <c r="C27" s="67">
         <v>9296766</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A28" s="78" t="s">
+      <c r="A28" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="79">
+      <c r="B28" s="67">
         <v>2730325</v>
       </c>
-      <c r="C28" s="79">
+      <c r="C28" s="67">
         <v>2730325</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A29" s="78" t="s">
+      <c r="A29" s="66" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="79">
+      <c r="B29" s="67">
         <v>4692095</v>
       </c>
-      <c r="C29" s="79">
+      <c r="C29" s="67">
         <v>4692089.46</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A30" s="78" t="s">
+      <c r="A30" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="79">
+      <c r="B30" s="67">
         <v>1653213</v>
       </c>
-      <c r="C30" s="79">
+      <c r="C30" s="67">
         <v>1652677</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A31" s="78" t="s">
+      <c r="A31" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="B31" s="79">
+      <c r="B31" s="67">
         <v>3301114</v>
       </c>
-      <c r="C31" s="79">
+      <c r="C31" s="67">
         <v>3301114</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A32" s="78" t="s">
+      <c r="A32" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="79">
+      <c r="B32" s="67">
         <v>22551603</v>
       </c>
-      <c r="C32" s="79">
+      <c r="C32" s="67">
         <v>21778540</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A33" s="78" t="s">
+      <c r="A33" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="79">
+      <c r="B33" s="67">
         <v>6554186</v>
       </c>
-      <c r="C33" s="79">
+      <c r="C33" s="67">
         <v>6554186</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A34" s="78" t="s">
+      <c r="A34" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="B34" s="79">
+      <c r="B34" s="67">
         <v>5492219</v>
       </c>
-      <c r="C34" s="79">
+      <c r="C34" s="67">
         <v>4283508</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A35" s="78" t="s">
+      <c r="A35" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="79">
+      <c r="B35" s="67">
         <v>8638087</v>
       </c>
-      <c r="C35" s="79">
+      <c r="C35" s="67">
         <v>8542014.6500000004</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A36" s="78" t="s">
+      <c r="A36" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="B36" s="79">
+      <c r="B36" s="67">
         <v>332487485.71000004</v>
       </c>
-      <c r="C36" s="79">
+      <c r="C36" s="67">
         <v>254062125.53000003</v>
       </c>
     </row>
@@ -2594,10 +2625,10 @@
   <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C37" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2613,1526 +2644,1527 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="58.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="33" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="48" customFormat="1" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:9" s="43" customFormat="1" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="16">
+        <v>11894913</v>
+      </c>
+      <c r="F2" s="42">
+        <v>44770</v>
+      </c>
+      <c r="G2" s="44">
+        <v>11782773</v>
+      </c>
+      <c r="H2" s="39" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="13">
+        <v>7900000</v>
+      </c>
+      <c r="F3" s="54">
+        <v>44481</v>
+      </c>
+      <c r="G3" s="56">
+        <f>6949908+457162+74808+37404</f>
+        <v>7519282</v>
+      </c>
+      <c r="H3" s="36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="17" t="s">
+      <c r="B4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="18">
-        <v>11894913</v>
-      </c>
-      <c r="F2" s="47">
-        <v>44770</v>
-      </c>
-      <c r="G2" s="49">
-        <v>11782773</v>
-      </c>
-      <c r="H2" s="44" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="11" t="s">
+      <c r="E4" s="12">
+        <v>10258000</v>
+      </c>
+      <c r="F4" s="17">
+        <v>44638</v>
+      </c>
+      <c r="G4" s="83">
+        <v>6027030.7999999998</v>
+      </c>
+      <c r="H4" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="36"/>
+    </row>
+    <row r="5" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="13">
+        <v>1144242</v>
+      </c>
+      <c r="F5" s="54">
+        <v>44418</v>
+      </c>
+      <c r="G5" s="84">
+        <v>1144242</v>
+      </c>
+      <c r="H5" s="62" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="13">
-        <v>10258000</v>
-      </c>
-      <c r="F3" s="19">
-        <v>44638</v>
-      </c>
-      <c r="G3" s="71">
-        <v>6027030.7999999998</v>
-      </c>
-      <c r="H3" s="41" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="52" t="s">
+      <c r="B6" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="9" t="s">
+      <c r="C6" s="46"/>
+      <c r="D6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E6" s="12">
         <v>1576793</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F6" s="81">
         <v>44851</v>
       </c>
-      <c r="G4" s="72">
+      <c r="G6" s="77">
         <v>92497</v>
       </c>
-      <c r="H4" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="41"/>
-    </row>
-    <row r="5" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="52" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="43">
-        <v>8058093</v>
-      </c>
-      <c r="F5" s="19"/>
-      <c r="H5" s="73" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="37">
-        <v>29107860</v>
-      </c>
-      <c r="F6" s="57">
-        <v>44782</v>
-      </c>
-      <c r="G6" s="68">
-        <v>15329692.93</v>
-      </c>
-      <c r="H6" s="53" t="s">
+      <c r="H6" s="47" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="36">
-        <v>9197974</v>
-      </c>
-      <c r="F7" s="58">
-        <v>44778</v>
-      </c>
-      <c r="G7" s="51">
-        <v>224976</v>
-      </c>
-      <c r="H7" s="41" t="s">
+      <c r="A7" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="13">
+        <v>1303508</v>
+      </c>
+      <c r="F7" s="55">
+        <v>44502</v>
+      </c>
+      <c r="G7" s="84">
+        <v>1303508</v>
+      </c>
+      <c r="H7" s="36" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="11" t="s">
-        <v>83</v>
+      <c r="A8" s="10" t="s">
+        <v>96</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="52" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="3">
-        <v>8407821.7100000009</v>
-      </c>
-      <c r="F8" s="4">
-        <v>44643</v>
-      </c>
-      <c r="G8" s="3">
-        <v>8182845.71</v>
+        <v>56</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="14">
+        <v>5507618</v>
+      </c>
+      <c r="F8" s="55">
+        <v>44489</v>
+      </c>
+      <c r="G8" s="57">
+        <f>196992+5230626</f>
+        <v>5427618</v>
       </c>
       <c r="H8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="11" t="s">
-        <v>84</v>
+      <c r="A9" s="10" t="s">
+        <v>97</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="14">
+        <v>978421</v>
+      </c>
+      <c r="F9" s="55">
+        <v>44491</v>
+      </c>
+      <c r="G9" s="56">
+        <f>292108+686313</f>
+        <v>978421</v>
+      </c>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="76">
+        <v>9197974</v>
+      </c>
+      <c r="F10" s="51">
+        <v>44778</v>
+      </c>
+      <c r="G10" s="86">
+        <v>224976</v>
+      </c>
+      <c r="H10" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="45" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="3">
+        <v>8407821.7100000009</v>
+      </c>
+      <c r="F11" s="4">
+        <v>44643</v>
+      </c>
+      <c r="G11" s="3">
+        <v>8182845.71</v>
+      </c>
+      <c r="H11" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="34"/>
+    </row>
+    <row r="12" spans="1:9" ht="34.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="14">
+        <v>15000000</v>
+      </c>
+      <c r="F12" s="55">
+        <v>44462</v>
+      </c>
+      <c r="G12" s="56">
+        <f>14600000+85612.5+44673.69</f>
+        <v>14730286.189999999</v>
+      </c>
+      <c r="H12" s="41" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="34.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9" t="s">
+      <c r="C13" s="7"/>
+      <c r="D13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E13" s="3">
         <v>12555809</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F13" s="4">
         <v>44638</v>
       </c>
-      <c r="G9" s="45">
+      <c r="G13" s="40">
         <f>6844818+349596+331058</f>
         <v>7525472</v>
       </c>
-      <c r="H9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="3">
-        <v>4100000</v>
-      </c>
-      <c r="F10" s="59"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="I10" s="50" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="55">
-        <v>8035407</v>
-      </c>
-      <c r="F11" s="59"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" s="38"/>
-    </row>
-    <row r="12" spans="1:9" ht="34.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="3">
-        <v>3000000</v>
-      </c>
-      <c r="F12" s="4">
-        <v>44551</v>
-      </c>
-      <c r="G12" s="3">
-        <v>1686683</v>
-      </c>
-      <c r="H12" s="46" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="34.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="3">
-        <v>8943548</v>
-      </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="69" t="s">
+      <c r="H13" s="60" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="11" t="s">
-        <v>88</v>
+      <c r="A14" s="10" t="s">
+        <v>82</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="3">
-        <v>542235</v>
-      </c>
-      <c r="F14" s="4">
-        <v>44551</v>
-      </c>
-      <c r="G14" s="3">
-        <v>542235</v>
+        <v>24</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="14">
+        <v>2211196</v>
+      </c>
+      <c r="F14" s="55">
+        <v>44462</v>
+      </c>
+      <c r="G14" s="56">
+        <f>1923741+80488+18469+86237+12446+12573.37</f>
+        <v>2133954.37</v>
       </c>
       <c r="H14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="11" t="s">
-        <v>88</v>
+      <c r="A15" s="10" t="s">
+        <v>83</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="3">
-        <v>4128053</v>
-      </c>
-      <c r="F15" s="4"/>
+        <v>4100000</v>
+      </c>
+      <c r="F15" s="52"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="70" t="s">
+      <c r="H15" s="61" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="11" t="s">
-        <v>89</v>
+      <c r="A16" s="10" t="s">
+        <v>83</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="3">
-        <v>2975917</v>
-      </c>
-      <c r="F16" s="4">
-        <v>44685</v>
-      </c>
-      <c r="G16" s="3">
-        <v>2975917</v>
+        <v>26</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="14">
+        <v>3959315</v>
+      </c>
+      <c r="F16" s="55">
+        <v>44511</v>
+      </c>
+      <c r="G16" s="56">
+        <f>2000000+107400+197400</f>
+        <v>2304800</v>
       </c>
       <c r="H16" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="11" t="s">
-        <v>90</v>
+      <c r="A17" t="s">
+        <v>105</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="14">
-        <v>23433350</v>
-      </c>
-      <c r="F17" s="60">
-        <v>44643</v>
-      </c>
-      <c r="G17" s="3">
-        <v>23433350</v>
+        <v>59</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="78">
+        <v>977007</v>
+      </c>
+      <c r="F17" s="55">
+        <v>44468</v>
+      </c>
+      <c r="G17" s="56">
+        <v>977007</v>
       </c>
       <c r="H17" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="11" t="s">
-        <v>90</v>
+      <c r="A18" s="10" t="s">
+        <v>98</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="78">
+        <v>978460</v>
+      </c>
+      <c r="F18" s="55">
+        <v>44489</v>
+      </c>
+      <c r="G18" s="56">
+        <v>978460</v>
+      </c>
+      <c r="H18" s="50" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="49">
+        <v>8035407</v>
+      </c>
+      <c r="F19" s="52"/>
+      <c r="G19" s="3"/>
+      <c r="H19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="28.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="78">
+        <v>2138482</v>
+      </c>
+      <c r="F20" s="55">
+        <v>44496</v>
+      </c>
+      <c r="G20" s="56">
+        <f>1686666.67+451815.42</f>
+        <v>2138482.09</v>
+      </c>
+      <c r="H20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="40.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="F21" s="4">
+        <v>44551</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1686683</v>
+      </c>
+      <c r="H21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="34.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="3">
+        <v>8943548</v>
+      </c>
+      <c r="F22" s="4"/>
+      <c r="G22" s="3"/>
+      <c r="H22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="14">
+        <v>4306517</v>
+      </c>
+      <c r="F23" s="55">
+        <v>44432</v>
+      </c>
+      <c r="G23" s="56">
+        <f>500000+2306517+200000+26944.5+15783.5+1300000</f>
+        <v>4349245</v>
+      </c>
+      <c r="H23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="14">
+        <v>4070028</v>
+      </c>
+      <c r="F24" s="55">
+        <v>44439</v>
+      </c>
+      <c r="G24" s="56">
+        <f>3982627+81401</f>
+        <v>4064028</v>
+      </c>
+      <c r="H24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="45.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="78">
+        <v>3105169</v>
+      </c>
+      <c r="F25" s="55">
+        <v>44511</v>
+      </c>
+      <c r="G25" s="56">
+        <f>124207+3377016+124206</f>
+        <v>3625429</v>
+      </c>
+      <c r="H25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="45.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="7"/>
+      <c r="D26" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="75">
+        <v>542235</v>
+      </c>
+      <c r="F26" s="4">
+        <v>44551</v>
+      </c>
+      <c r="G26" s="3">
+        <v>542235</v>
+      </c>
+      <c r="H26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="40.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="75">
+        <v>4128053</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="3"/>
+      <c r="H27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="78">
+        <v>1493213</v>
+      </c>
+      <c r="F28" s="55">
+        <v>44505</v>
+      </c>
+      <c r="G28" s="56">
+        <f>779887.65+589325+70000+12201</f>
+        <v>1451413.65</v>
+      </c>
+      <c r="H28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="3">
+        <v>2975917</v>
+      </c>
+      <c r="F29" s="4">
+        <v>44685</v>
+      </c>
+      <c r="G29" s="3">
+        <v>2975917</v>
+      </c>
+      <c r="H29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" s="14">
+        <v>3500000</v>
+      </c>
+      <c r="F30" s="55">
+        <v>44462</v>
+      </c>
+      <c r="G30" s="58">
+        <v>3500000</v>
+      </c>
+      <c r="H30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C31" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D31" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="40">
+      <c r="E31" s="3">
+        <v>23433350</v>
+      </c>
+      <c r="F31" s="53">
+        <v>44643</v>
+      </c>
+      <c r="G31" s="3">
+        <v>23433350</v>
+      </c>
+      <c r="H31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" s="68" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="68" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="38">
         <v>6216901</v>
       </c>
-      <c r="F18" s="60">
+      <c r="F32" s="87">
         <v>44805</v>
       </c>
-      <c r="G18" s="54">
+      <c r="G32" s="88">
         <v>3581632</v>
       </c>
-      <c r="H18" s="56" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="B19" s="6" t="s">
+      <c r="H32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="10"/>
+      <c r="D33" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" s="14">
+        <v>9995380</v>
+      </c>
+      <c r="F33" s="55">
+        <v>44484</v>
+      </c>
+      <c r="G33" s="57">
+        <f>5124130+4871251+60661.74+366320.37</f>
+        <v>10422363.109999999</v>
+      </c>
+      <c r="H33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9" t="s">
+      <c r="C34" s="68"/>
+      <c r="D34" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E34" s="3">
         <v>2180890</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F34" s="4">
         <v>44665</v>
       </c>
-      <c r="G19" s="45">
+      <c r="G34" s="40">
         <f>942269+586829</f>
         <v>1529098</v>
       </c>
-      <c r="H19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="28.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B20" s="6" t="s">
+      <c r="H34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="10"/>
+      <c r="D35" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E35" s="14">
+        <v>2745604</v>
+      </c>
+      <c r="F35" s="55">
+        <v>44547</v>
+      </c>
+      <c r="G35" s="56">
+        <v>31079.25</v>
+      </c>
+      <c r="H35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="68" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="3">
+        <v>5763000</v>
+      </c>
+      <c r="F36" s="4">
+        <v>44699</v>
+      </c>
+      <c r="G36" s="3">
+        <v>5760333</v>
+      </c>
+      <c r="H36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="10"/>
+      <c r="D37" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E37" s="14">
+        <v>3536420</v>
+      </c>
+      <c r="F37" s="55">
+        <v>44533</v>
+      </c>
+      <c r="G37" s="56">
+        <f>1124355+2412078</f>
+        <v>3536433</v>
+      </c>
+      <c r="H37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A38" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="10"/>
+      <c r="D38" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E38" s="14">
+        <v>1380115</v>
+      </c>
+      <c r="F38" s="55">
+        <v>44484</v>
+      </c>
+      <c r="G38" s="56">
+        <v>1380115</v>
+      </c>
+      <c r="H38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="74" t="s">
+      <c r="C39" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D39" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E39" s="3">
         <v>1977284</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F39" s="4">
         <v>44631</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G39" s="3">
         <v>1977284</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H39" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="40.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="B21" s="6" t="s">
+    <row r="40" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" s="10"/>
+      <c r="D40" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E40" s="14">
+        <v>967690</v>
+      </c>
+      <c r="F40" s="55">
+        <v>44468</v>
+      </c>
+      <c r="G40" s="56">
+        <f>252647+715040</f>
+        <v>967687</v>
+      </c>
+      <c r="H40" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C41" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D41" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E41" s="3">
         <v>5552930</v>
       </c>
-      <c r="F21" s="39">
+      <c r="F41" s="35">
         <v>44754</v>
       </c>
-      <c r="G21" s="45">
+      <c r="G41" s="40">
         <f>2784017.52+2375672.8+152280+240750</f>
         <v>5552720.3200000003</v>
       </c>
-      <c r="H21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="34.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="B22" s="6" t="s">
+      <c r="H41" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" s="10"/>
+      <c r="D42" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E42" s="14">
+        <v>5100000</v>
+      </c>
+      <c r="F42" s="55">
+        <v>44502</v>
+      </c>
+      <c r="G42" s="56">
+        <f>2275285+2824715</f>
+        <v>5100000</v>
+      </c>
+      <c r="H42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A43" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C43" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D43" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E43" s="3">
         <v>2800000</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F43" s="4">
         <v>44685</v>
       </c>
-      <c r="G22" s="75">
+      <c r="G43" s="63">
         <v>2584985</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H43" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="9" t="s">
+    <row r="44" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" s="10"/>
+      <c r="D44" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E44" s="14">
+        <v>2988882</v>
+      </c>
+      <c r="F44" s="55">
+        <v>44491</v>
+      </c>
+      <c r="G44" s="56">
+        <f>963663+970391+757400+58062+17250+29031+65590</f>
+        <v>2861387</v>
+      </c>
+      <c r="H44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" s="10"/>
+      <c r="D45" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E45" s="14">
+        <v>2730325</v>
+      </c>
+      <c r="F45" s="55">
+        <v>44510</v>
+      </c>
+      <c r="G45" s="56">
+        <f>1365162.5+1365162.5</f>
+        <v>2730325</v>
+      </c>
+      <c r="H45" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A46" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" s="68"/>
+      <c r="D46" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="3">
-        <v>5763000</v>
-      </c>
-      <c r="F23" s="4">
-        <v>44699</v>
-      </c>
-      <c r="G23" s="3">
-        <v>5760333</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="E46" s="3">
+        <v>4692095</v>
+      </c>
+      <c r="F46" s="4">
+        <v>44692</v>
+      </c>
+      <c r="G46" s="3">
+        <v>4692089.46</v>
+      </c>
+      <c r="H46" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9" t="s">
+    <row r="47" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" s="68"/>
+      <c r="D47" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="3">
-        <v>4692095</v>
-      </c>
-      <c r="F24" s="4">
-        <v>44692</v>
-      </c>
-      <c r="G24" s="3">
-        <v>4692089.46</v>
-      </c>
-      <c r="H24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="45.7" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="14">
+      <c r="E47" s="3">
         <v>1653213</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F47" s="4">
         <v>44726</v>
       </c>
-      <c r="G25" s="45">
+      <c r="G47" s="40">
         <f>752120+900557</f>
         <v>1652677</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H47" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="45.7" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" s="6" t="s">
+    <row r="48" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B48" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="9" t="s">
+      <c r="C48" s="68"/>
+      <c r="D48" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="40">
+      <c r="E48" s="74">
         <v>3301114</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F48" s="4">
         <v>44775</v>
       </c>
-      <c r="G26" s="54">
+      <c r="G48" s="48">
         <v>3301114</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H48" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="40.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="7">
-        <v>4899111</v>
-      </c>
-      <c r="F27" s="4">
-        <v>44665</v>
-      </c>
-      <c r="G27" s="3">
-        <v>4899111</v>
-      </c>
-      <c r="H27" t="s">
+    <row r="49" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49" s="69" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="D49" s="72" t="s">
+        <v>14</v>
+      </c>
+      <c r="E49" s="74">
+        <v>8058093</v>
+      </c>
+      <c r="F49" s="4"/>
+      <c r="G49" s="85"/>
+      <c r="H49" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="7">
-        <v>10900000</v>
-      </c>
-      <c r="F28" s="4">
-        <v>44747</v>
-      </c>
-      <c r="G28" s="42">
-        <v>10126937</v>
-      </c>
-      <c r="H28" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="3">
-        <v>3000000</v>
-      </c>
-      <c r="F29" s="4">
-        <v>44617</v>
-      </c>
-      <c r="G29" s="3">
-        <v>3000000</v>
-      </c>
-      <c r="H29" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="3">
-        <v>1208710</v>
-      </c>
-      <c r="F30" s="4"/>
-      <c r="G30" s="3"/>
-      <c r="H30" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="3">
-        <v>6717249</v>
-      </c>
-      <c r="F31" s="4">
-        <v>44719</v>
-      </c>
-      <c r="G31" s="76">
-        <v>6621177</v>
-      </c>
-      <c r="H31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="5" t="s">
+    <row r="50" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" s="10"/>
+      <c r="D50" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E32" s="15">
-        <v>7900000</v>
-      </c>
-      <c r="F32" s="61">
-        <v>44481</v>
-      </c>
-      <c r="G32" s="63">
-        <f>6949908+457162+74808+37404</f>
-        <v>7519282</v>
-      </c>
-      <c r="H32" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="11"/>
-      <c r="D33" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E33" s="16">
-        <v>1144242</v>
-      </c>
-      <c r="F33" s="62">
-        <v>44418</v>
-      </c>
-      <c r="G33" s="64">
-        <v>1144242</v>
-      </c>
-      <c r="H33" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E34" s="16">
-        <v>5507618</v>
-      </c>
-      <c r="F34" s="62">
-        <v>44489</v>
-      </c>
-      <c r="G34" s="65">
-        <f>196992+5230626</f>
-        <v>5427618</v>
-      </c>
-      <c r="H34" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E35" s="16">
-        <v>1303508</v>
-      </c>
-      <c r="F35" s="62">
+      <c r="E50" s="14">
+        <v>5000000</v>
+      </c>
+      <c r="F50" s="55">
         <v>44502</v>
       </c>
-      <c r="G35" s="64">
-        <v>1303508</v>
-      </c>
-      <c r="H35" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E36" s="16">
-        <v>5000000</v>
-      </c>
-      <c r="F36" s="62">
-        <v>44502</v>
-      </c>
-      <c r="G36" s="64">
+      <c r="G50" s="56">
         <f>4000000+700000+300000</f>
         <v>5000000</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H50" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B37" s="6" t="s">
+    <row r="51" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>103</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51" s="68"/>
+      <c r="D51" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="79">
+        <v>4899111</v>
+      </c>
+      <c r="F51" s="4">
+        <v>44665</v>
+      </c>
+      <c r="G51" s="3">
+        <v>4899111</v>
+      </c>
+      <c r="H51" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>103</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C52" s="68"/>
+      <c r="D52" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" s="79">
+        <v>10900000</v>
+      </c>
+      <c r="F52" s="4">
+        <v>44747</v>
+      </c>
+      <c r="G52" s="37">
+        <v>10126937</v>
+      </c>
+      <c r="H52" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>103</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C53" s="10"/>
+      <c r="D53" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E53" s="14">
+        <v>6752492</v>
+      </c>
+      <c r="F53" s="55">
+        <v>44439</v>
+      </c>
+      <c r="G53" s="56">
+        <v>6752492</v>
+      </c>
+      <c r="H53" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A54" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C54" s="68"/>
+      <c r="D54" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="F54" s="4">
+        <v>44617</v>
+      </c>
+      <c r="G54" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="H54" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A55" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C55" s="10"/>
+      <c r="D55" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E55" s="14">
+        <v>3554186</v>
+      </c>
+      <c r="F55" s="55">
+        <v>44418</v>
+      </c>
+      <c r="G55" s="56">
+        <f>3554186</f>
+        <v>3554186</v>
+      </c>
+      <c r="H55" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>104</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C56" s="68" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="3">
+        <v>1208710</v>
+      </c>
+      <c r="F56" s="4"/>
+      <c r="G56" s="3"/>
+      <c r="H56" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>104</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C57" s="10"/>
+      <c r="D57" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E57" s="14">
+        <v>4283509</v>
+      </c>
+      <c r="F57" s="55">
+        <v>44505</v>
+      </c>
+      <c r="G57" s="56">
+        <f>1043077+3240431</f>
+        <v>4283508</v>
+      </c>
+      <c r="H57" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A58" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C58" s="68"/>
+      <c r="D58" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="3">
+        <v>6717249</v>
+      </c>
+      <c r="F58" s="4">
+        <v>44719</v>
+      </c>
+      <c r="G58" s="64">
+        <v>6621177</v>
+      </c>
+      <c r="H58" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A59" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C59" s="10"/>
+      <c r="D59" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E59" s="14">
+        <v>1920838</v>
+      </c>
+      <c r="F59" s="55">
+        <v>44489</v>
+      </c>
+      <c r="G59" s="57">
+        <f>637595+472476+810766.65</f>
+        <v>1920837.65</v>
+      </c>
+      <c r="H59" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>106</v>
+      </c>
+      <c r="B60" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="C37" s="11"/>
-      <c r="D37" s="5" t="s">
+      <c r="C60" s="70"/>
+      <c r="D60" s="72" t="s">
+        <v>14</v>
+      </c>
+      <c r="E60" s="73">
+        <v>29107860</v>
+      </c>
+      <c r="F60" s="80">
+        <v>44782</v>
+      </c>
+      <c r="G60" s="82">
+        <v>15329692.93</v>
+      </c>
+      <c r="H60" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>106</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C61" s="10"/>
+      <c r="D61" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E37" s="16">
+      <c r="E61" s="14">
         <v>13252291</v>
       </c>
-      <c r="F37" s="62">
+      <c r="F61" s="55">
         <v>44474</v>
       </c>
-      <c r="G37" s="64">
+      <c r="G61" s="56">
         <f>3009307+8507891+1667401</f>
         <v>13184599</v>
       </c>
-      <c r="H37" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C38" s="11"/>
-      <c r="D38" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E38" s="16">
-        <v>2628307</v>
-      </c>
-      <c r="F38" s="62">
-        <v>44487</v>
-      </c>
-      <c r="G38" s="65">
-        <v>2628307</v>
-      </c>
-      <c r="H38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C39" s="11"/>
-      <c r="D39" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E39" s="16">
-        <v>978421</v>
-      </c>
-      <c r="F39" s="62">
-        <v>44491</v>
-      </c>
-      <c r="G39" s="64">
-        <f>292108+686313</f>
-        <v>978421</v>
-      </c>
-      <c r="H39" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C40" s="11"/>
-      <c r="D40" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E40" s="16">
-        <v>15000000</v>
-      </c>
-      <c r="F40" s="62">
-        <v>44462</v>
-      </c>
-      <c r="G40" s="64">
-        <f>14600000+85612.5+44673.69</f>
-        <v>14730286.189999999</v>
-      </c>
-      <c r="H40" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C41" s="11"/>
-      <c r="D41" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E41" s="16">
-        <v>977007</v>
-      </c>
-      <c r="F41" s="62">
-        <v>44468</v>
-      </c>
-      <c r="G41" s="64">
-        <v>977007</v>
-      </c>
-      <c r="H41" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C42" s="11"/>
-      <c r="D42" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E42" s="16">
-        <v>2211196</v>
-      </c>
-      <c r="F42" s="62">
-        <v>44462</v>
-      </c>
-      <c r="G42" s="64">
-        <f>1923741+80488+18469+86237+12446+12573.37</f>
-        <v>2133954.37</v>
-      </c>
-      <c r="H42" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C43" s="11"/>
-      <c r="D43" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E43" s="16">
-        <v>3959315</v>
-      </c>
-      <c r="F43" s="62">
-        <v>44511</v>
-      </c>
-      <c r="G43" s="64">
-        <f>2000000+107400+197400</f>
-        <v>2304800</v>
-      </c>
-      <c r="H43" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C44" s="11"/>
-      <c r="D44" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E44" s="16">
-        <v>978460</v>
-      </c>
-      <c r="F44" s="62">
-        <v>44489</v>
-      </c>
-      <c r="G44" s="64">
-        <v>978460</v>
-      </c>
-      <c r="H44" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C45" s="11"/>
-      <c r="D45" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E45" s="16">
-        <v>2138482</v>
-      </c>
-      <c r="F45" s="62">
-        <v>44496</v>
-      </c>
-      <c r="G45" s="64">
-        <f>1686666.67+451815.42</f>
-        <v>2138482.09</v>
-      </c>
-      <c r="H45" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C46" s="11"/>
-      <c r="D46" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E46" s="16">
-        <v>4306517</v>
-      </c>
-      <c r="F46" s="62">
-        <v>44432</v>
-      </c>
-      <c r="G46" s="64">
-        <f>500000+2306517+200000+26944.5+15783.5+1300000</f>
-        <v>4349245</v>
-      </c>
-      <c r="H46" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C47" s="11"/>
-      <c r="D47" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E47" s="16">
-        <v>4070028</v>
-      </c>
-      <c r="F47" s="62">
-        <v>44439</v>
-      </c>
-      <c r="G47" s="64">
-        <f>3982627+81401</f>
-        <v>4064028</v>
-      </c>
-      <c r="H47" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C48" s="11"/>
-      <c r="D48" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E48" s="16">
-        <v>1493213</v>
-      </c>
-      <c r="F48" s="62">
-        <v>44505</v>
-      </c>
-      <c r="G48" s="64">
-        <f>779887.65+589325+70000+12201</f>
-        <v>1451413.65</v>
-      </c>
-      <c r="H48" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C49" s="11"/>
-      <c r="D49" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E49" s="16">
-        <v>3105169</v>
-      </c>
-      <c r="F49" s="62">
-        <v>44511</v>
-      </c>
-      <c r="G49" s="64">
-        <f>124207+3377016+124206</f>
-        <v>3625429</v>
-      </c>
-      <c r="H49" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C50" s="11"/>
-      <c r="D50" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E50" s="16">
-        <v>3500000</v>
-      </c>
-      <c r="F50" s="62">
-        <v>44462</v>
-      </c>
-      <c r="G50" s="66">
-        <v>3500000</v>
-      </c>
-      <c r="H50" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C51" s="11"/>
-      <c r="D51" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E51" s="16">
-        <v>9995380</v>
-      </c>
-      <c r="F51" s="62">
-        <v>44484</v>
-      </c>
-      <c r="G51" s="65">
-        <f>5124130+4871251+60661.74+366320.37</f>
-        <v>10422363.109999999</v>
-      </c>
-      <c r="H51" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C52" s="11"/>
-      <c r="D52" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E52" s="16">
-        <v>2745604</v>
-      </c>
-      <c r="F52" s="62">
-        <v>44547</v>
-      </c>
-      <c r="G52" s="64">
-        <v>31079.25</v>
-      </c>
-      <c r="H52" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C53" s="11"/>
-      <c r="D53" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E53" s="16">
-        <v>1380115</v>
-      </c>
-      <c r="F53" s="62">
-        <v>44484</v>
-      </c>
-      <c r="G53" s="64">
-        <v>1380115</v>
-      </c>
-      <c r="H53" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C54" s="11"/>
-      <c r="D54" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E54" s="16">
-        <v>967690</v>
-      </c>
-      <c r="F54" s="62">
-        <v>44468</v>
-      </c>
-      <c r="G54" s="64">
-        <f>252647+715040</f>
-        <v>967687</v>
-      </c>
-      <c r="H54" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C55" s="11"/>
-      <c r="D55" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E55" s="16">
-        <v>5100000</v>
-      </c>
-      <c r="F55" s="62">
-        <v>44502</v>
-      </c>
-      <c r="G55" s="64">
-        <f>2275285+2824715</f>
-        <v>5100000</v>
-      </c>
-      <c r="H55" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C56" s="11"/>
-      <c r="D56" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E56" s="16">
-        <v>2988882</v>
-      </c>
-      <c r="F56" s="62">
-        <v>44491</v>
-      </c>
-      <c r="G56" s="64">
-        <f>963663+970391+757400+58062+17250+29031+65590</f>
-        <v>2861387</v>
-      </c>
-      <c r="H56" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C57" s="11"/>
-      <c r="D57" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E57" s="16">
-        <v>3536420</v>
-      </c>
-      <c r="F57" s="62">
-        <v>44533</v>
-      </c>
-      <c r="G57" s="64">
-        <f>1124355+2412078</f>
-        <v>3536433</v>
-      </c>
-      <c r="H57" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B58" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C58" s="11"/>
-      <c r="D58" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E58" s="16">
-        <v>2730325</v>
-      </c>
-      <c r="F58" s="62">
-        <v>44510</v>
-      </c>
-      <c r="G58" s="64">
-        <f>1365162.5+1365162.5</f>
-        <v>2730325</v>
-      </c>
-      <c r="H58" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C59" s="11"/>
-      <c r="D59" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E59" s="16">
-        <v>6752492</v>
-      </c>
-      <c r="F59" s="62">
-        <v>44439</v>
-      </c>
-      <c r="G59" s="64">
-        <v>6752492</v>
-      </c>
-      <c r="H59" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A60" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C60" s="11"/>
-      <c r="D60" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E60" s="16">
-        <v>3554186</v>
-      </c>
-      <c r="F60" s="62">
-        <v>44418</v>
-      </c>
-      <c r="G60" s="64">
-        <f>3554186</f>
-        <v>3554186</v>
-      </c>
-      <c r="H60" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A61" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C61" s="11"/>
-      <c r="D61" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E61" s="16">
-        <v>4283509</v>
-      </c>
-      <c r="F61" s="62">
-        <v>44505</v>
-      </c>
-      <c r="G61" s="64">
-        <f>1043077+3240431</f>
-        <v>4283508</v>
-      </c>
       <c r="H61" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="11" t="s">
-        <v>99</v>
+      <c r="A62" t="s">
+        <v>107</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C62" s="11"/>
+        <v>57</v>
+      </c>
+      <c r="C62" s="10"/>
       <c r="D62" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E62" s="16">
-        <v>1920838</v>
-      </c>
-      <c r="F62" s="62">
-        <v>44489</v>
-      </c>
-      <c r="G62" s="65">
-        <f>637595+472476+810766.65</f>
-        <v>1920837.65</v>
+      <c r="E62" s="14">
+        <v>2628307</v>
+      </c>
+      <c r="F62" s="55">
+        <v>44487</v>
+      </c>
+      <c r="G62" s="57">
+        <v>2628307</v>
       </c>
       <c r="H62" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G63" s="41"/>
+      <c r="G63" s="36"/>
     </row>
   </sheetData>
   <protectedRanges>
@@ -4187,46 +4219,46 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="20"/>
+      <c r="B2" s="18"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="19"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="26"/>
+      <c r="B4" s="24"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="22"/>
+      <c r="B5" s="20"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="24"/>
+      <c r="B6" s="22"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="23"/>
+      <c r="B7" s="21"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="25"/>
+      <c r="B8" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4238,21 +4270,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001F87334A6AC30D4EA6021977FA7E2445" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="13eff9136b4917bb459ad9c1db870f6d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b370a6fa-a798-42e0-969d-19c284d8683f" xmlns:ns3="62ca1376-8bea-4949-825e-fec085c3924e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="60e7197df19c7150b1ba0c3bfe00adf4" ns2:_="" ns3:_="">
     <xsd:import namespace="b370a6fa-a798-42e0-969d-19c284d8683f"/>
@@ -4469,15 +4492,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DDCF067-268F-4A3C-A288-B4575E68AABA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{752D7A7F-0D65-4907-85A4-76807BF1350E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4489,7 +4513,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D681DB6D-9136-4740-BD99-737079D2FCBE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4506,4 +4530,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DDCF067-268F-4A3C-A288-B4575E68AABA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
week of 24 November commit
</commit_message>
<xml_diff>
--- a/data/input/base_financing_cds.xlsx
+++ b/data/input/base_financing_cds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg-my.sharepoint.com/personal/panlilioj_who_int/Documents/covid19_vaccination_analysis/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{26E979B5-FA10-4638-B812-BC8073066A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1EAC695-6716-47B8-B630-1C1E6A15BF86}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{26E979B5-FA10-4638-B812-BC8073066A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA4A0608-5229-472A-B245-28F527B07A05}"/>
   <bookViews>
-    <workbookView xWindow="2175" yWindow="2175" windowWidth="16230" windowHeight="9998" activeTab="1" xr2:uid="{FD644F38-BFEB-4730-9E59-BCD9CF33A41F}"/>
+    <workbookView xWindow="5768" yWindow="2910" windowWidth="16230" windowHeight="9998" activeTab="1" xr2:uid="{FD644F38-BFEB-4730-9E59-BCD9CF33A41F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId4"/>
+    <pivotCache cacheId="18" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -362,100 +362,100 @@
     <t xml:space="preserve">Sum of Amount approved </t>
   </si>
   <si>
+    <t>CAF</t>
+  </si>
+  <si>
+    <t>AFG</t>
+  </si>
+  <si>
+    <t>BFA</t>
+  </si>
+  <si>
+    <t>CMR</t>
+  </si>
+  <si>
+    <t>TCD</t>
+  </si>
+  <si>
+    <t>DJI</t>
+  </si>
+  <si>
+    <t>ETH</t>
+  </si>
+  <si>
+    <t>GHA</t>
+  </si>
+  <si>
+    <t>GIN</t>
+  </si>
+  <si>
+    <t>GNB</t>
+  </si>
+  <si>
+    <t>HTI</t>
+  </si>
+  <si>
+    <t>KEN</t>
+  </si>
+  <si>
+    <t>MDG</t>
+  </si>
+  <si>
+    <t>MWI</t>
+  </si>
+  <si>
+    <t>MLI</t>
+  </si>
+  <si>
+    <t>NER</t>
+  </si>
+  <si>
+    <t>NGA</t>
+  </si>
+  <si>
+    <t>PNG</t>
+  </si>
+  <si>
+    <t>SEN</t>
+  </si>
+  <si>
+    <t>SLE</t>
+  </si>
+  <si>
+    <t>SOM</t>
+  </si>
+  <si>
+    <t>SSD</t>
+  </si>
+  <si>
+    <t>SDN</t>
+  </si>
+  <si>
+    <t>TZA</t>
+  </si>
+  <si>
+    <t>UGA</t>
+  </si>
+  <si>
+    <t>ZMB</t>
+  </si>
+  <si>
     <t>ISO</t>
   </si>
   <si>
-    <t>AFG</t>
-  </si>
-  <si>
-    <t>BFA</t>
-  </si>
-  <si>
-    <t>CAF</t>
-  </si>
-  <si>
-    <t>TCD</t>
-  </si>
-  <si>
     <t>COD</t>
   </si>
   <si>
-    <t>ETH</t>
-  </si>
-  <si>
-    <t>GHA</t>
-  </si>
-  <si>
-    <t>GIN</t>
-  </si>
-  <si>
-    <t>HTI</t>
-  </si>
-  <si>
-    <t>KEN</t>
-  </si>
-  <si>
-    <t>MWI</t>
-  </si>
-  <si>
-    <t>NER</t>
-  </si>
-  <si>
-    <t>NGA</t>
-  </si>
-  <si>
-    <t>PNG</t>
-  </si>
-  <si>
-    <t>SLE</t>
-  </si>
-  <si>
-    <t>SOM</t>
-  </si>
-  <si>
-    <t>SSD</t>
-  </si>
-  <si>
-    <t>SDN</t>
+    <t>CIV</t>
+  </si>
+  <si>
+    <t>GMB</t>
   </si>
   <si>
     <t>SYR</t>
   </si>
   <si>
-    <t>TZA</t>
-  </si>
-  <si>
-    <t>UGA</t>
-  </si>
-  <si>
     <t>YEM</t>
-  </si>
-  <si>
-    <t>ZMB</t>
-  </si>
-  <si>
-    <t>CMR</t>
-  </si>
-  <si>
-    <t>CIV</t>
-  </si>
-  <si>
-    <t>DJI</t>
-  </si>
-  <si>
-    <t>GMB</t>
-  </si>
-  <si>
-    <t>GNB</t>
-  </si>
-  <si>
-    <t>MDG</t>
-  </si>
-  <si>
-    <t>MLI</t>
-  </si>
-  <si>
-    <t>SEN</t>
   </si>
 </sst>
 </file>
@@ -738,7 +738,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -755,9 +755,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -780,7 +777,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -819,18 +815,14 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="12" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="169" fontId="6" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="12" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -850,7 +842,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -862,9 +853,6 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="6" fillId="13" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -895,16 +883,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="13" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="40" fontId="0" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="40" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -912,6 +893,49 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="12" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="12" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="40% - Accent4 5" xfId="4" xr:uid="{BBE1C5CD-EB81-46A5-A1EB-6EEB64CB90EF}"/>
@@ -1666,7 +1690,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C9206A13-E1F8-4BA4-9E83-D2C707B1EEF4}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C9206A13-E1F8-4BA4-9E83-D2C707B1EEF4}" name="PivotTable1" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:C36" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
@@ -2189,7 +2213,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="65" t="s">
         <v>72</v>
       </c>
       <c r="B1" t="s">
@@ -2200,387 +2224,387 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="79">
+      <c r="B2" s="67">
         <v>19794913</v>
       </c>
-      <c r="C2" s="79">
+      <c r="C2" s="67">
         <v>19302055</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="79">
+      <c r="B3" s="67">
         <v>11402242</v>
       </c>
-      <c r="C3" s="79">
+      <c r="C3" s="67">
         <v>7171272.7999999998</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="79">
+      <c r="B4" s="67">
         <v>5507618</v>
       </c>
-      <c r="C4" s="79">
+      <c r="C4" s="67">
         <v>5427618</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="79">
+      <c r="B5" s="67">
         <v>2880301</v>
       </c>
-      <c r="C5" s="79">
+      <c r="C5" s="67">
         <v>1396005</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="79">
+      <c r="B6" s="67">
         <v>13058093</v>
       </c>
-      <c r="C6" s="79">
+      <c r="C6" s="67">
         <v>5000000</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="78" t="s">
+      <c r="A7" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="79">
+      <c r="B7" s="67">
         <v>42360151</v>
       </c>
-      <c r="C7" s="79">
+      <c r="C7" s="67">
         <v>28514291.93</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" s="78" t="s">
+      <c r="A8" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="79">
+      <c r="B8" s="67">
         <v>2628307</v>
       </c>
-      <c r="C8" s="79">
+      <c r="C8" s="67">
         <v>2628307</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" s="78" t="s">
+      <c r="A9" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="79">
+      <c r="B9" s="67">
         <v>978421</v>
       </c>
-      <c r="C9" s="79">
+      <c r="C9" s="67">
         <v>978421</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" s="78" t="s">
+      <c r="A10" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="79">
+      <c r="B10" s="67">
         <v>32605795.710000001</v>
       </c>
-      <c r="C10" s="79">
+      <c r="C10" s="67">
         <v>23138107.899999999</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" s="78" t="s">
+      <c r="A11" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="79">
+      <c r="B11" s="67">
         <v>977007</v>
       </c>
-      <c r="C11" s="79">
+      <c r="C11" s="67">
         <v>977007</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12" s="78" t="s">
+      <c r="A12" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="79">
+      <c r="B12" s="67">
         <v>14767005</v>
       </c>
-      <c r="C12" s="79">
+      <c r="C12" s="67">
         <v>9659426.370000001</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13" s="78" t="s">
+      <c r="A13" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="79">
+      <c r="B13" s="67">
         <v>8059315</v>
       </c>
-      <c r="C13" s="79">
+      <c r="C13" s="67">
         <v>2304800</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A14" s="78" t="s">
+      <c r="A14" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="79">
+      <c r="B14" s="67">
         <v>978460</v>
       </c>
-      <c r="C14" s="79">
+      <c r="C14" s="67">
         <v>978460</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" s="78" t="s">
+      <c r="A15" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="79">
+      <c r="B15" s="67">
         <v>10173889</v>
       </c>
-      <c r="C15" s="79">
+      <c r="C15" s="67">
         <v>2138482.09</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A16" s="78" t="s">
+      <c r="A16" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="79">
+      <c r="B16" s="67">
         <v>16250065</v>
       </c>
-      <c r="C16" s="79">
+      <c r="C16" s="67">
         <v>6035928</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A17" s="78" t="s">
+      <c r="A17" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="79">
+      <c r="B17" s="67">
         <v>4070028</v>
       </c>
-      <c r="C17" s="79">
+      <c r="C17" s="67">
         <v>4064028</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" s="78" t="s">
+      <c r="A18" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="79">
+      <c r="B18" s="67">
         <v>6163501</v>
       </c>
-      <c r="C18" s="79">
+      <c r="C18" s="67">
         <v>1993648.65</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A19" s="78" t="s">
+      <c r="A19" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="79">
+      <c r="B19" s="67">
         <v>3105169</v>
       </c>
-      <c r="C19" s="79">
+      <c r="C19" s="67">
         <v>3625429</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A20" s="78" t="s">
+      <c r="A20" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="79">
+      <c r="B20" s="67">
         <v>6475917</v>
       </c>
-      <c r="C20" s="79">
+      <c r="C20" s="67">
         <v>6475917</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21" s="78" t="s">
+      <c r="A21" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="79">
+      <c r="B21" s="67">
         <v>39645631</v>
       </c>
-      <c r="C21" s="79">
+      <c r="C21" s="67">
         <v>37437345.109999999</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" s="78" t="s">
+      <c r="A22" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="79">
+      <c r="B22" s="67">
         <v>4926494</v>
       </c>
-      <c r="C22" s="79">
+      <c r="C22" s="67">
         <v>1560177.25</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A23" s="78" t="s">
+      <c r="A23" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="79">
+      <c r="B23" s="67">
         <v>1380115</v>
       </c>
-      <c r="C23" s="79">
+      <c r="C23" s="67">
         <v>1380115</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A24" s="78" t="s">
+      <c r="A24" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="79">
+      <c r="B24" s="67">
         <v>2944974</v>
       </c>
-      <c r="C24" s="79">
+      <c r="C24" s="67">
         <v>2944971</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A25" s="78" t="s">
+      <c r="A25" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="79">
+      <c r="B25" s="67">
         <v>10652930</v>
       </c>
-      <c r="C25" s="79">
+      <c r="C25" s="67">
         <v>10652720.32</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A26" s="78" t="s">
+      <c r="A26" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="79">
+      <c r="B26" s="67">
         <v>5788882</v>
       </c>
-      <c r="C26" s="79">
+      <c r="C26" s="67">
         <v>5446372</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A27" s="78" t="s">
+      <c r="A27" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="79">
+      <c r="B27" s="67">
         <v>9299420</v>
       </c>
-      <c r="C27" s="79">
+      <c r="C27" s="67">
         <v>9296766</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A28" s="78" t="s">
+      <c r="A28" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="79">
+      <c r="B28" s="67">
         <v>2730325</v>
       </c>
-      <c r="C28" s="79">
+      <c r="C28" s="67">
         <v>2730325</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A29" s="78" t="s">
+      <c r="A29" s="66" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="79">
+      <c r="B29" s="67">
         <v>4692095</v>
       </c>
-      <c r="C29" s="79">
+      <c r="C29" s="67">
         <v>4692089.46</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A30" s="78" t="s">
+      <c r="A30" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="79">
+      <c r="B30" s="67">
         <v>1653213</v>
       </c>
-      <c r="C30" s="79">
+      <c r="C30" s="67">
         <v>1652677</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A31" s="78" t="s">
+      <c r="A31" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="B31" s="79">
+      <c r="B31" s="67">
         <v>3301114</v>
       </c>
-      <c r="C31" s="79">
+      <c r="C31" s="67">
         <v>3301114</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A32" s="78" t="s">
+      <c r="A32" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="79">
+      <c r="B32" s="67">
         <v>22551603</v>
       </c>
-      <c r="C32" s="79">
+      <c r="C32" s="67">
         <v>21778540</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A33" s="78" t="s">
+      <c r="A33" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="79">
+      <c r="B33" s="67">
         <v>6554186</v>
       </c>
-      <c r="C33" s="79">
+      <c r="C33" s="67">
         <v>6554186</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A34" s="78" t="s">
+      <c r="A34" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="B34" s="79">
+      <c r="B34" s="67">
         <v>5492219</v>
       </c>
-      <c r="C34" s="79">
+      <c r="C34" s="67">
         <v>4283508</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A35" s="78" t="s">
+      <c r="A35" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="79">
+      <c r="B35" s="67">
         <v>8638087</v>
       </c>
-      <c r="C35" s="79">
+      <c r="C35" s="67">
         <v>8542014.6500000004</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A36" s="78" t="s">
+      <c r="A36" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="B36" s="79">
+      <c r="B36" s="67">
         <v>332487485.71000004</v>
       </c>
-      <c r="C36" s="79">
+      <c r="C36" s="67">
         <v>254062125.53000003</v>
       </c>
     </row>
@@ -2594,10 +2618,10 @@
   <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2613,1295 +2637,1303 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="58.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="42" customFormat="1" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="16">
+        <v>11894913</v>
+      </c>
+      <c r="F2" s="41">
+        <v>44770</v>
+      </c>
+      <c r="G2" s="43">
+        <v>11782773</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="13">
+        <v>7900000</v>
+      </c>
+      <c r="F3" s="53">
+        <v>44481</v>
+      </c>
+      <c r="G3" s="56">
+        <f>6949908+457162+74808+37404</f>
+        <v>7519282</v>
+      </c>
+      <c r="H3" s="36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="12">
+        <v>10258000</v>
+      </c>
+      <c r="F4" s="17">
+        <v>44638</v>
+      </c>
+      <c r="G4" s="84">
+        <v>6027030.7999999998</v>
+      </c>
+      <c r="H4" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="36"/>
+    </row>
+    <row r="5" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="13">
+        <v>1144242</v>
+      </c>
+      <c r="F5" s="53">
+        <v>44418</v>
+      </c>
+      <c r="G5" s="85">
+        <v>1144242</v>
+      </c>
+      <c r="H5" s="62" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="13">
+        <v>5507618</v>
+      </c>
+      <c r="F6" s="79">
+        <v>44489</v>
+      </c>
+      <c r="G6" s="81">
+        <f>196992+5230626</f>
+        <v>5427618</v>
+      </c>
+      <c r="H6" s="46" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="35" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="48" customFormat="1" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="18">
-        <v>11894913</v>
-      </c>
-      <c r="F2" s="47">
-        <v>44770</v>
-      </c>
-      <c r="G2" s="49">
-        <v>11782773</v>
-      </c>
-      <c r="H2" s="44" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="13">
-        <v>10258000</v>
-      </c>
-      <c r="F3" s="19">
-        <v>44638</v>
-      </c>
-      <c r="G3" s="71">
-        <v>6027030.7999999998</v>
-      </c>
-      <c r="H3" s="41" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="52" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="9" t="s">
+      <c r="C7" s="45"/>
+      <c r="D7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E7" s="12">
         <v>1576793</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F7" s="4">
         <v>44851</v>
       </c>
-      <c r="G4" s="72">
+      <c r="G7" s="83">
         <v>92497</v>
       </c>
-      <c r="H4" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="41"/>
-    </row>
-    <row r="5" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="52" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="43">
-        <v>8058093</v>
-      </c>
-      <c r="F5" s="19"/>
-      <c r="H5" s="73" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="37">
-        <v>29107860</v>
-      </c>
-      <c r="F6" s="57">
-        <v>44782</v>
-      </c>
-      <c r="G6" s="68">
-        <v>15329692.93</v>
-      </c>
-      <c r="H6" s="53" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="36">
-        <v>9197974</v>
-      </c>
-      <c r="F7" s="58">
-        <v>44778</v>
-      </c>
-      <c r="G7" s="51">
-        <v>224976</v>
-      </c>
-      <c r="H7" s="41" t="s">
+      <c r="H7" s="36" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" s="52" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="3">
-        <v>8407821.7100000009</v>
-      </c>
-      <c r="F8" s="4">
-        <v>44643</v>
-      </c>
-      <c r="G8" s="3">
-        <v>8182845.71</v>
+        <v>13</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="14">
+        <v>1303508</v>
+      </c>
+      <c r="F8" s="54">
+        <v>44502</v>
+      </c>
+      <c r="G8" s="56">
+        <v>1303508</v>
       </c>
       <c r="H8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="69" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="77">
+        <v>8058093</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="86"/>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="14">
+        <v>5000000</v>
+      </c>
+      <c r="F10" s="54">
+        <v>44502</v>
+      </c>
+      <c r="G10" s="56">
+        <f>4000000+700000+300000</f>
+        <v>5000000</v>
+      </c>
+      <c r="H10" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="69" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" s="45"/>
+      <c r="D11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="75">
+        <v>29107860</v>
+      </c>
+      <c r="F11" s="78">
+        <v>44782</v>
+      </c>
+      <c r="G11" s="80">
+        <v>15329692.93</v>
+      </c>
+      <c r="H11" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="34"/>
+    </row>
+    <row r="12" spans="1:9" ht="34.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="14">
+        <v>13252291</v>
+      </c>
+      <c r="F12" s="54">
+        <v>44474</v>
+      </c>
+      <c r="G12" s="56">
+        <f>3009307+8507891+1667401</f>
+        <v>13184599</v>
+      </c>
+      <c r="H12" s="40" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="34.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="14">
+        <v>2628307</v>
+      </c>
+      <c r="F13" s="54">
+        <v>44487</v>
+      </c>
+      <c r="G13" s="57">
+        <v>2628307</v>
+      </c>
+      <c r="H13" s="60" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="14">
+        <v>978421</v>
+      </c>
+      <c r="F14" s="54">
+        <v>44491</v>
+      </c>
+      <c r="G14" s="56">
+        <f>292108+686313</f>
+        <v>978421</v>
+      </c>
+      <c r="H14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="76">
+        <v>9197974</v>
+      </c>
+      <c r="F15" s="50">
+        <v>44778</v>
+      </c>
+      <c r="G15" s="82">
+        <v>224976</v>
+      </c>
+      <c r="H15" s="61" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="3">
+        <v>8407821.7100000009</v>
+      </c>
+      <c r="F16" s="4">
+        <v>44643</v>
+      </c>
+      <c r="G16" s="3">
+        <v>8182845.71</v>
+      </c>
+      <c r="H16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="72">
+        <v>15000000</v>
+      </c>
+      <c r="F17" s="54">
+        <v>44462</v>
+      </c>
+      <c r="G17" s="56">
+        <f>14600000+85612.5+44673.69</f>
+        <v>14730286.189999999</v>
+      </c>
+      <c r="H17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="72">
+        <v>977007</v>
+      </c>
+      <c r="F18" s="54">
+        <v>44468</v>
+      </c>
+      <c r="G18" s="56">
+        <v>977007</v>
+      </c>
+      <c r="H18" s="49" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B19" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9" t="s">
+      <c r="C19" s="7"/>
+      <c r="D19" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E19" s="3">
         <v>12555809</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F19" s="4">
         <v>44638</v>
       </c>
-      <c r="G9" s="45">
+      <c r="G19" s="39">
         <f>6844818+349596+331058</f>
         <v>7525472</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="6" t="s">
+    <row r="20" spans="1:8" ht="28.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="72">
+        <v>2211196</v>
+      </c>
+      <c r="F20" s="54">
+        <v>44462</v>
+      </c>
+      <c r="G20" s="56">
+        <f>1923741+80488+18469+86237+12446+12573.37</f>
+        <v>2133954.37</v>
+      </c>
+      <c r="H20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="40.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B21" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9" t="s">
+      <c r="C21" s="7"/>
+      <c r="D21" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E21" s="3">
         <v>4100000</v>
       </c>
-      <c r="F10" s="59"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="I10" s="50" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="6" t="s">
+      <c r="F21" s="51"/>
+      <c r="G21" s="3"/>
+      <c r="H21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="34.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="14">
+        <v>3959315</v>
+      </c>
+      <c r="F22" s="54">
+        <v>44511</v>
+      </c>
+      <c r="G22" s="56">
+        <f>2000000+107400+197400</f>
+        <v>2304800</v>
+      </c>
+      <c r="H22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="14">
+        <v>978460</v>
+      </c>
+      <c r="F23" s="54">
+        <v>44489</v>
+      </c>
+      <c r="G23" s="56">
+        <v>978460</v>
+      </c>
+      <c r="H23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9" t="s">
+      <c r="B24" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="55">
+      <c r="E24" s="48">
         <v>8035407</v>
       </c>
-      <c r="F11" s="59"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" s="38"/>
-    </row>
-    <row r="12" spans="1:9" ht="34.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="6" t="s">
+      <c r="F24" s="51"/>
+      <c r="G24" s="3"/>
+      <c r="H24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="45.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="72">
+        <v>2138482</v>
+      </c>
+      <c r="F25" s="54">
+        <v>44496</v>
+      </c>
+      <c r="G25" s="56">
+        <f>1686666.67+451815.42</f>
+        <v>2138482.09</v>
+      </c>
+      <c r="H25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="45.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9" t="s">
+      <c r="B26" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="7"/>
+      <c r="D26" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E26" s="74">
         <v>3000000</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F26" s="4">
         <v>44551</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G26" s="3">
         <v>1686683</v>
       </c>
-      <c r="H12" s="46" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="34.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="6" t="s">
+      <c r="H26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="40.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9" t="s">
+      <c r="B27" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="7"/>
+      <c r="D27" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E27" s="74">
         <v>8943548</v>
       </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="69" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="6" t="s">
+      <c r="F27" s="4"/>
+      <c r="G27" s="3"/>
+      <c r="H27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="72">
+        <v>4306517</v>
+      </c>
+      <c r="F28" s="54">
+        <v>44432</v>
+      </c>
+      <c r="G28" s="56">
+        <f>500000+2306517+200000+26944.5+15783.5+1300000</f>
+        <v>4349245</v>
+      </c>
+      <c r="H28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="14">
+        <v>4070028</v>
+      </c>
+      <c r="F29" s="54">
+        <v>44439</v>
+      </c>
+      <c r="G29" s="56">
+        <f>3982627+81401</f>
+        <v>4064028</v>
+      </c>
+      <c r="H29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9" t="s">
+      <c r="B30" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E30" s="3">
         <v>542235</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F30" s="4">
         <v>44551</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G30" s="3">
         <v>542235</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="3">
+        <v>4128053</v>
+      </c>
+      <c r="F31" s="4"/>
+      <c r="G31" s="3"/>
+      <c r="H31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="68" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" s="10"/>
+      <c r="D32" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E32" s="13">
+        <v>1493213</v>
+      </c>
+      <c r="F32" s="53">
+        <v>44505</v>
+      </c>
+      <c r="G32" s="55">
+        <f>779887.65+589325+70000+12201</f>
+        <v>1451413.65</v>
+      </c>
+      <c r="H32" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" s="8" t="s">
+    <row r="33" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="10"/>
+      <c r="D33" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" s="14">
+        <v>3105169</v>
+      </c>
+      <c r="F33" s="54">
+        <v>44511</v>
+      </c>
+      <c r="G33" s="56">
+        <f>124207+3377016+124206</f>
+        <v>3625429</v>
+      </c>
+      <c r="H33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" s="68"/>
+      <c r="D34" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="3">
+        <v>2975917</v>
+      </c>
+      <c r="F34" s="4">
+        <v>44685</v>
+      </c>
+      <c r="G34" s="3">
+        <v>2975917</v>
+      </c>
+      <c r="H34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="10"/>
+      <c r="D35" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E35" s="14">
+        <v>3500000</v>
+      </c>
+      <c r="F35" s="54">
+        <v>44462</v>
+      </c>
+      <c r="G35" s="58">
+        <v>3500000</v>
+      </c>
+      <c r="H35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D36" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="3">
-        <v>4128053</v>
-      </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="70" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9" t="s">
+      <c r="E36" s="3">
+        <v>23433350</v>
+      </c>
+      <c r="F36" s="52">
+        <v>44643</v>
+      </c>
+      <c r="G36" s="3">
+        <v>23433350</v>
+      </c>
+      <c r="H36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" s="68" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="3">
-        <v>2975917</v>
-      </c>
-      <c r="F16" s="4">
-        <v>44685</v>
-      </c>
-      <c r="G16" s="3">
-        <v>2975917</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="E37" s="77">
+        <v>6216901</v>
+      </c>
+      <c r="F37" s="52">
+        <v>44805</v>
+      </c>
+      <c r="G37" s="47">
+        <v>3581632</v>
+      </c>
+      <c r="H37" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="6" t="s">
+    <row r="38" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A38" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="9" t="s">
+      <c r="B38" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" s="10"/>
+      <c r="D38" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E38" s="14">
+        <v>9995380</v>
+      </c>
+      <c r="F38" s="54">
+        <v>44484</v>
+      </c>
+      <c r="G38" s="57">
+        <f>5124130+4871251+60661.74+366320.37</f>
+        <v>10422363.109999999</v>
+      </c>
+      <c r="H38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" s="68"/>
+      <c r="D39" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="14">
-        <v>23433350</v>
-      </c>
-      <c r="F17" s="60">
-        <v>44643</v>
-      </c>
-      <c r="G17" s="3">
-        <v>23433350</v>
-      </c>
-      <c r="H17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="40">
-        <v>6216901</v>
-      </c>
-      <c r="F18" s="60">
-        <v>44805</v>
-      </c>
-      <c r="G18" s="54">
-        <v>3581632</v>
-      </c>
-      <c r="H18" s="56" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="3">
+      <c r="E39" s="3">
         <v>2180890</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F39" s="4">
         <v>44665</v>
       </c>
-      <c r="G19" s="45">
+      <c r="G39" s="39">
         <f>942269+586829</f>
         <v>1529098</v>
       </c>
-      <c r="H19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="28.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="6" t="s">
+      <c r="H39" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" s="10"/>
+      <c r="D40" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E40" s="14">
+        <v>2745604</v>
+      </c>
+      <c r="F40" s="54">
+        <v>44547</v>
+      </c>
+      <c r="G40" s="56">
+        <v>31079.25</v>
+      </c>
+      <c r="H40" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" s="10"/>
+      <c r="D41" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E41" s="14">
+        <v>1380115</v>
+      </c>
+      <c r="F41" s="54">
+        <v>44484</v>
+      </c>
+      <c r="G41" s="56">
+        <v>1380115</v>
+      </c>
+      <c r="H41" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="C20" s="74" t="s">
+      <c r="B42" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C42" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D42" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E42" s="3">
         <v>1977284</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F42" s="4">
         <v>44631</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G42" s="3">
         <v>1977284</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H42" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="40.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="6" t="s">
+    <row r="43" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A43" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" s="10"/>
+      <c r="D43" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E43" s="14">
+        <v>967690</v>
+      </c>
+      <c r="F43" s="54">
+        <v>44468</v>
+      </c>
+      <c r="G43" s="56">
+        <f>252647+715040</f>
+        <v>967687</v>
+      </c>
+      <c r="H43" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C21" s="8" t="s">
+      <c r="B44" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D44" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E44" s="3">
         <v>5552930</v>
       </c>
-      <c r="F21" s="39">
+      <c r="F44" s="35">
         <v>44754</v>
       </c>
-      <c r="G21" s="45">
+      <c r="G44" s="39">
         <f>2784017.52+2375672.8+152280+240750</f>
         <v>5552720.3200000003</v>
       </c>
-      <c r="H21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="34.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="6" t="s">
+      <c r="H44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C45" s="10"/>
+      <c r="D45" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E45" s="14">
+        <v>5100000</v>
+      </c>
+      <c r="F45" s="54">
+        <v>44502</v>
+      </c>
+      <c r="G45" s="56">
+        <f>2275285+2824715</f>
+        <v>5100000</v>
+      </c>
+      <c r="H45" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A46" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C22" s="8" t="s">
+      <c r="B46" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C46" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D46" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E46" s="3">
         <v>2800000</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F46" s="4">
         <v>44685</v>
       </c>
-      <c r="G22" s="75">
+      <c r="G46" s="63">
         <v>2584985</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H46" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="6" t="s">
+    <row r="47" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47" s="10"/>
+      <c r="D47" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E47" s="14">
+        <v>2988882</v>
+      </c>
+      <c r="F47" s="54">
+        <v>44491</v>
+      </c>
+      <c r="G47" s="56">
+        <f>963663+970391+757400+58062+17250+29031+65590</f>
+        <v>2861387</v>
+      </c>
+      <c r="H47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C23" s="8" t="s">
+      <c r="B48" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D48" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E48" s="3">
         <v>5763000</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F48" s="4">
         <v>44699</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G48" s="3">
         <v>5760333</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H48" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="6" t="s">
+    <row r="49" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" s="10"/>
+      <c r="D49" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E49" s="14">
+        <v>3536420</v>
+      </c>
+      <c r="F49" s="54">
+        <v>44533</v>
+      </c>
+      <c r="G49" s="56">
+        <f>1124355+2412078</f>
+        <v>3536433</v>
+      </c>
+      <c r="H49" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C50" s="10"/>
+      <c r="D50" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E50" s="14">
+        <v>2730325</v>
+      </c>
+      <c r="F50" s="54">
+        <v>44510</v>
+      </c>
+      <c r="G50" s="56">
+        <f>1365162.5+1365162.5</f>
+        <v>2730325</v>
+      </c>
+      <c r="H50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9" t="s">
+      <c r="B51" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C51" s="68"/>
+      <c r="D51" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E51" s="3">
         <v>4692095</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F51" s="4">
         <v>44692</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G51" s="3">
         <v>4692089.46</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H51" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="45.7" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="6" t="s">
+    <row r="52" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A52" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9" t="s">
+      <c r="B52" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C52" s="68"/>
+      <c r="D52" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E52" s="3">
         <v>1653213</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F52" s="4">
         <v>44726</v>
       </c>
-      <c r="G25" s="45">
+      <c r="G52" s="39">
         <f>752120+900557</f>
         <v>1652677</v>
       </c>
-      <c r="H25" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="45.7" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="40">
-        <v>3301114</v>
-      </c>
-      <c r="F26" s="4">
-        <v>44775</v>
-      </c>
-      <c r="G26" s="54">
-        <v>3301114</v>
-      </c>
-      <c r="H26" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="40.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="7">
-        <v>4899111</v>
-      </c>
-      <c r="F27" s="4">
-        <v>44665</v>
-      </c>
-      <c r="G27" s="3">
-        <v>4899111</v>
-      </c>
-      <c r="H27" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="7">
-        <v>10900000</v>
-      </c>
-      <c r="F28" s="4">
-        <v>44747</v>
-      </c>
-      <c r="G28" s="42">
-        <v>10126937</v>
-      </c>
-      <c r="H28" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="3">
-        <v>3000000</v>
-      </c>
-      <c r="F29" s="4">
-        <v>44617</v>
-      </c>
-      <c r="G29" s="3">
-        <v>3000000</v>
-      </c>
-      <c r="H29" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="3">
-        <v>1208710</v>
-      </c>
-      <c r="F30" s="4"/>
-      <c r="G30" s="3"/>
-      <c r="H30" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="3">
-        <v>6717249</v>
-      </c>
-      <c r="F31" s="4">
-        <v>44719</v>
-      </c>
-      <c r="G31" s="76">
-        <v>6621177</v>
-      </c>
-      <c r="H31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E32" s="15">
-        <v>7900000</v>
-      </c>
-      <c r="F32" s="61">
-        <v>44481</v>
-      </c>
-      <c r="G32" s="63">
-        <f>6949908+457162+74808+37404</f>
-        <v>7519282</v>
-      </c>
-      <c r="H32" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C33" s="11"/>
-      <c r="D33" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E33" s="16">
-        <v>1144242</v>
-      </c>
-      <c r="F33" s="62">
-        <v>44418</v>
-      </c>
-      <c r="G33" s="64">
-        <v>1144242</v>
-      </c>
-      <c r="H33" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E34" s="16">
-        <v>5507618</v>
-      </c>
-      <c r="F34" s="62">
-        <v>44489</v>
-      </c>
-      <c r="G34" s="65">
-        <f>196992+5230626</f>
-        <v>5427618</v>
-      </c>
-      <c r="H34" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E35" s="16">
-        <v>1303508</v>
-      </c>
-      <c r="F35" s="62">
-        <v>44502</v>
-      </c>
-      <c r="G35" s="64">
-        <v>1303508</v>
-      </c>
-      <c r="H35" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E36" s="16">
-        <v>5000000</v>
-      </c>
-      <c r="F36" s="62">
-        <v>44502</v>
-      </c>
-      <c r="G36" s="64">
-        <f>4000000+700000+300000</f>
-        <v>5000000</v>
-      </c>
-      <c r="H36" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="C37" s="11"/>
-      <c r="D37" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E37" s="16">
-        <v>13252291</v>
-      </c>
-      <c r="F37" s="62">
-        <v>44474</v>
-      </c>
-      <c r="G37" s="64">
-        <f>3009307+8507891+1667401</f>
-        <v>13184599</v>
-      </c>
-      <c r="H37" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="C38" s="11"/>
-      <c r="D38" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E38" s="16">
-        <v>2628307</v>
-      </c>
-      <c r="F38" s="62">
-        <v>44487</v>
-      </c>
-      <c r="G38" s="65">
-        <v>2628307</v>
-      </c>
-      <c r="H38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="C39" s="11"/>
-      <c r="D39" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E39" s="16">
-        <v>978421</v>
-      </c>
-      <c r="F39" s="62">
-        <v>44491</v>
-      </c>
-      <c r="G39" s="64">
-        <f>292108+686313</f>
-        <v>978421</v>
-      </c>
-      <c r="H39" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="C40" s="11"/>
-      <c r="D40" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E40" s="16">
-        <v>15000000</v>
-      </c>
-      <c r="F40" s="62">
-        <v>44462</v>
-      </c>
-      <c r="G40" s="64">
-        <f>14600000+85612.5+44673.69</f>
-        <v>14730286.189999999</v>
-      </c>
-      <c r="H40" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="C41" s="11"/>
-      <c r="D41" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E41" s="16">
-        <v>977007</v>
-      </c>
-      <c r="F41" s="62">
-        <v>44468</v>
-      </c>
-      <c r="G41" s="64">
-        <v>977007</v>
-      </c>
-      <c r="H41" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="C42" s="11"/>
-      <c r="D42" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E42" s="16">
-        <v>2211196</v>
-      </c>
-      <c r="F42" s="62">
-        <v>44462</v>
-      </c>
-      <c r="G42" s="64">
-        <f>1923741+80488+18469+86237+12446+12573.37</f>
-        <v>2133954.37</v>
-      </c>
-      <c r="H42" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="C43" s="11"/>
-      <c r="D43" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E43" s="16">
-        <v>3959315</v>
-      </c>
-      <c r="F43" s="62">
-        <v>44511</v>
-      </c>
-      <c r="G43" s="64">
-        <f>2000000+107400+197400</f>
-        <v>2304800</v>
-      </c>
-      <c r="H43" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C44" s="11"/>
-      <c r="D44" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E44" s="16">
-        <v>978460</v>
-      </c>
-      <c r="F44" s="62">
-        <v>44489</v>
-      </c>
-      <c r="G44" s="64">
-        <v>978460</v>
-      </c>
-      <c r="H44" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C45" s="11"/>
-      <c r="D45" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E45" s="16">
-        <v>2138482</v>
-      </c>
-      <c r="F45" s="62">
-        <v>44496</v>
-      </c>
-      <c r="G45" s="64">
-        <f>1686666.67+451815.42</f>
-        <v>2138482.09</v>
-      </c>
-      <c r="H45" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="C46" s="11"/>
-      <c r="D46" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E46" s="16">
-        <v>4306517</v>
-      </c>
-      <c r="F46" s="62">
-        <v>44432</v>
-      </c>
-      <c r="G46" s="64">
-        <f>500000+2306517+200000+26944.5+15783.5+1300000</f>
-        <v>4349245</v>
-      </c>
-      <c r="H46" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="C47" s="11"/>
-      <c r="D47" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E47" s="16">
-        <v>4070028</v>
-      </c>
-      <c r="F47" s="62">
-        <v>44439</v>
-      </c>
-      <c r="G47" s="64">
-        <f>3982627+81401</f>
-        <v>4064028</v>
-      </c>
-      <c r="H47" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="C48" s="11"/>
-      <c r="D48" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E48" s="16">
-        <v>1493213</v>
-      </c>
-      <c r="F48" s="62">
-        <v>44505</v>
-      </c>
-      <c r="G48" s="64">
-        <f>779887.65+589325+70000+12201</f>
-        <v>1451413.65</v>
-      </c>
-      <c r="H48" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B49" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="C49" s="11"/>
-      <c r="D49" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E49" s="16">
-        <v>3105169</v>
-      </c>
-      <c r="F49" s="62">
-        <v>44511</v>
-      </c>
-      <c r="G49" s="64">
-        <f>124207+3377016+124206</f>
-        <v>3625429</v>
-      </c>
-      <c r="H49" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="C50" s="11"/>
-      <c r="D50" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E50" s="16">
-        <v>3500000</v>
-      </c>
-      <c r="F50" s="62">
-        <v>44462</v>
-      </c>
-      <c r="G50" s="66">
-        <v>3500000</v>
-      </c>
-      <c r="H50" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B51" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="C51" s="11"/>
-      <c r="D51" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E51" s="16">
-        <v>9995380</v>
-      </c>
-      <c r="F51" s="62">
-        <v>44484</v>
-      </c>
-      <c r="G51" s="65">
-        <f>5124130+4871251+60661.74+366320.37</f>
-        <v>10422363.109999999</v>
-      </c>
-      <c r="H51" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="C52" s="11"/>
-      <c r="D52" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E52" s="16">
-        <v>2745604</v>
-      </c>
-      <c r="F52" s="62">
-        <v>44547</v>
-      </c>
-      <c r="G52" s="64">
-        <v>31079.25</v>
-      </c>
       <c r="H52" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B53" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="C53" s="11"/>
-      <c r="D53" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E53" s="16">
-        <v>1380115</v>
-      </c>
-      <c r="F53" s="62">
-        <v>44484</v>
-      </c>
-      <c r="G53" s="64">
-        <v>1380115</v>
+        <v>49</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C53" s="68"/>
+      <c r="D53" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="77">
+        <v>3301114</v>
+      </c>
+      <c r="F53" s="4">
+        <v>44775</v>
+      </c>
+      <c r="G53" s="47">
+        <v>3301114</v>
       </c>
       <c r="H53" t="s">
         <v>10</v>
@@ -3909,24 +3941,23 @@
     </row>
     <row r="54" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B54" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="C54" s="11"/>
-      <c r="D54" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E54" s="16">
-        <v>967690</v>
-      </c>
-      <c r="F54" s="62">
-        <v>44468</v>
-      </c>
-      <c r="G54" s="64">
-        <f>252647+715040</f>
-        <v>967687</v>
+        <v>50</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C54" s="68"/>
+      <c r="D54" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="73">
+        <v>4899111</v>
+      </c>
+      <c r="F54" s="4">
+        <v>44665</v>
+      </c>
+      <c r="G54" s="3">
+        <v>4899111</v>
       </c>
       <c r="H54" t="s">
         <v>10</v>
@@ -3934,24 +3965,23 @@
     </row>
     <row r="55" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B55" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C55" s="11"/>
-      <c r="D55" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E55" s="16">
-        <v>5100000</v>
-      </c>
-      <c r="F55" s="62">
-        <v>44502</v>
-      </c>
-      <c r="G55" s="64">
-        <f>2275285+2824715</f>
-        <v>5100000</v>
+        <v>50</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C55" s="68"/>
+      <c r="D55" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="73">
+        <v>10900000</v>
+      </c>
+      <c r="F55" s="4">
+        <v>44747</v>
+      </c>
+      <c r="G55" s="37">
+        <v>10126937</v>
       </c>
       <c r="H55" t="s">
         <v>10</v>
@@ -3959,24 +3989,23 @@
     </row>
     <row r="56" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B56" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C56" s="11"/>
+        <v>50</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C56" s="10"/>
       <c r="D56" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E56" s="16">
-        <v>2988882</v>
-      </c>
-      <c r="F56" s="62">
-        <v>44491</v>
-      </c>
-      <c r="G56" s="64">
-        <f>963663+970391+757400+58062+17250+29031+65590</f>
-        <v>2861387</v>
+      <c r="E56" s="14">
+        <v>6752492</v>
+      </c>
+      <c r="F56" s="54">
+        <v>44439</v>
+      </c>
+      <c r="G56" s="56">
+        <v>6752492</v>
       </c>
       <c r="H56" t="s">
         <v>10</v>
@@ -3984,49 +4013,48 @@
     </row>
     <row r="57" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B57" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C57" s="11"/>
-      <c r="D57" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E57" s="16">
-        <v>3536420</v>
-      </c>
-      <c r="F57" s="62">
-        <v>44533</v>
-      </c>
-      <c r="G57" s="64">
-        <f>1124355+2412078</f>
-        <v>3536433</v>
+        <v>51</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C57" s="68"/>
+      <c r="D57" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="F57" s="4">
+        <v>44617</v>
+      </c>
+      <c r="G57" s="3">
+        <v>3000000</v>
       </c>
       <c r="H57" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B58" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C58" s="11"/>
+      <c r="A58" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C58" s="10"/>
       <c r="D58" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E58" s="16">
-        <v>2730325</v>
-      </c>
-      <c r="F58" s="62">
-        <v>44510</v>
-      </c>
-      <c r="G58" s="64">
-        <f>1365162.5+1365162.5</f>
-        <v>2730325</v>
+      <c r="E58" s="14">
+        <v>3554186</v>
+      </c>
+      <c r="F58" s="54">
+        <v>44418</v>
+      </c>
+      <c r="G58" s="56">
+        <f>3554186</f>
+        <v>3554186</v>
       </c>
       <c r="H58" t="s">
         <v>10</v>
@@ -4034,48 +4062,46 @@
     </row>
     <row r="59" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B59" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C59" s="11"/>
-      <c r="D59" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E59" s="16">
-        <v>6752492</v>
-      </c>
-      <c r="F59" s="62">
-        <v>44439</v>
-      </c>
-      <c r="G59" s="64">
-        <v>6752492</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C59" s="68" t="s">
+        <v>17</v>
+      </c>
+      <c r="D59" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="3">
+        <v>1208710</v>
+      </c>
+      <c r="F59" s="4"/>
+      <c r="G59" s="3"/>
       <c r="H59" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B60" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="C60" s="11"/>
+        <v>52</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C60" s="10"/>
       <c r="D60" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E60" s="16">
-        <v>3554186</v>
-      </c>
-      <c r="F60" s="62">
-        <v>44418</v>
-      </c>
-      <c r="G60" s="64">
-        <f>3554186</f>
-        <v>3554186</v>
+      <c r="E60" s="14">
+        <v>4283509</v>
+      </c>
+      <c r="F60" s="54">
+        <v>44505</v>
+      </c>
+      <c r="G60" s="56">
+        <f>1043077+3240431</f>
+        <v>4283508</v>
       </c>
       <c r="H60" t="s">
         <v>10</v>
@@ -4083,24 +4109,23 @@
     </row>
     <row r="61" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B61" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C61" s="11"/>
-      <c r="D61" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E61" s="16">
-        <v>4283509</v>
-      </c>
-      <c r="F61" s="62">
-        <v>44505</v>
+        <v>54</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C61" s="68"/>
+      <c r="D61" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="3">
+        <v>6717249</v>
+      </c>
+      <c r="F61" s="4">
+        <v>44719</v>
       </c>
       <c r="G61" s="64">
-        <f>1043077+3240431</f>
-        <v>4283508</v>
+        <v>6621177</v>
       </c>
       <c r="H61" t="s">
         <v>10</v>
@@ -4110,20 +4135,20 @@
       <c r="A62" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B62" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="C62" s="11"/>
+      <c r="B62" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C62" s="10"/>
       <c r="D62" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E62" s="16">
+      <c r="E62" s="14">
         <v>1920838</v>
       </c>
-      <c r="F62" s="62">
+      <c r="F62" s="54">
         <v>44489</v>
       </c>
-      <c r="G62" s="65">
+      <c r="G62" s="57">
         <f>637595+472476+810766.65</f>
         <v>1920837.65</v>
       </c>
@@ -4132,13 +4157,17 @@
       </c>
     </row>
     <row r="63" spans="1:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G63" s="41"/>
+      <c r="G63" s="36"/>
     </row>
   </sheetData>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="5Pc32SC9sKkOjch19iqZ+4Sh/UoLAdcgth1Gu1etoNQWZUfyNRyCcl196pqkoqf+mmoJ5yYFtcl02lDyXOP2sw==" saltValue="RazBueVJ8Os5LSXRduEbJw==" spinCount="100000" sqref="G32:G62" name="Range1_20"/>
   </protectedRanges>
-  <autoFilter ref="A1:G62" xr:uid="{684A2C1B-6B86-42B3-8147-0A75E163F9A5}"/>
+  <autoFilter ref="A1:G62" xr:uid="{684A2C1B-6B86-42B3-8147-0A75E163F9A5}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G62">
+      <sortCondition ref="A1:A62"/>
+    </sortState>
+  </autoFilter>
   <conditionalFormatting sqref="G32 G36:G37 G61 G56:G58 G52 G48:G49 G45:G46 G42:G43 G40">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="notEqual">
       <formula>"$h5:$h85"</formula>
@@ -4187,46 +4216,46 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="20"/>
+      <c r="B2" s="18"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="19"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="26"/>
+      <c r="B4" s="24"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="22"/>
+      <c r="B5" s="20"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="24"/>
+      <c r="B6" s="22"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="23"/>
+      <c r="B7" s="21"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="25"/>
+      <c r="B8" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4455,12 +4484,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4469,8 +4492,14 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D681DB6D-9136-4740-BD99-737079D2FCBE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45849AC2-01FA-4BC4-8DC7-B5EB49E54271}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -4489,6 +4518,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DDCF067-268F-4A3C-A288-B4575E68AABA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{752D7A7F-0D65-4907-85A4-76807BF1350E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4498,12 +4535,4 @@
     <ds:schemaRef ds:uri="55894003-98dc-4f3e-8669-85b90bdbcc8c"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DDCF067-268F-4A3C-A288-B4575E68AABA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>